<commit_message>
add miniFlySong and rig photos
</commit_message>
<xml_diff>
--- a/96ChannelRecordingRig.xlsx
+++ b/96ChannelRecordingRig.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sawtelles\Documents\GitHub\FlySong\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69AB5732-F34E-46C0-9BA5-4158A2D85A81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5C14766-262E-468C-9701-0C51BE371F16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="750" windowWidth="25005" windowHeight="14250" activeTab="2" xr2:uid="{0B008E79-2D1D-4383-A393-19DDE4F60BB8}"/>
+    <workbookView xWindow="1860" yWindow="1125" windowWidth="27630" windowHeight="14250" activeTab="2" xr2:uid="{0B008E79-2D1D-4383-A393-19DDE4F60BB8}"/>
   </bookViews>
   <sheets>
     <sheet name="Top Level" sheetId="1" r:id="rId1"/>
@@ -1108,9 +1108,6 @@
     <t>ePlastics</t>
   </si>
   <si>
-    <t xml:space="preserve"> 2447 White</t>
-  </si>
-  <si>
     <t>MB12</t>
   </si>
   <si>
@@ -1352,6 +1349,9 @@
   </si>
   <si>
     <t>Serial cable assembly</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2447 White 1/16" thick</t>
   </si>
 </sst>
 </file>
@@ -1488,9 +1488,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1528,7 +1528,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1634,7 +1634,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1776,7 +1776,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1788,7 +1788,7 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="42.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1990,22 +1990,22 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C9" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="F9" t="s">
         <v>15</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="H9" s="1">
         <v>59.62</v>
       </c>
       <c r="J9" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -2013,16 +2013,16 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C10" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F10" t="s">
         <v>15</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="H10" s="1">
         <v>25.34</v>
@@ -2033,22 +2033,22 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
+        <v>378</v>
+      </c>
+      <c r="C11" t="s">
         <v>379</v>
-      </c>
-      <c r="C11" t="s">
-        <v>380</v>
       </c>
       <c r="F11" t="s">
         <v>15</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="H11" s="1">
         <v>17.239999999999998</v>
       </c>
       <c r="J11" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -2071,7 +2071,7 @@
         <v>15</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="H12" s="1">
         <v>7.71</v>
@@ -2276,7 +2276,7 @@
         <v>58</v>
       </c>
       <c r="E19" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="F19" t="s">
         <v>10</v>
@@ -2351,10 +2351,10 @@
         <v>2</v>
       </c>
       <c r="B23" t="s">
+        <v>387</v>
+      </c>
+      <c r="C23" t="s">
         <v>388</v>
-      </c>
-      <c r="C23" t="s">
-        <v>389</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -2436,7 +2436,7 @@
   <sheetData>
     <row r="1" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="H1" s="12"/>
     </row>
@@ -2454,13 +2454,13 @@
         <v>3</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F3" s="13" t="s">
         <v>5</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="H3" s="12" t="s">
         <v>73</v>
@@ -2477,22 +2477,22 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C4" t="s">
+        <v>391</v>
+      </c>
+      <c r="D4" t="s">
         <v>392</v>
       </c>
-      <c r="D4" t="s">
-        <v>393</v>
-      </c>
       <c r="E4" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="F4" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>396</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>397</v>
       </c>
       <c r="H4" s="1">
         <v>850</v>
@@ -2507,16 +2507,16 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C5" t="s">
+        <v>397</v>
+      </c>
+      <c r="F5" t="s">
+        <v>395</v>
+      </c>
+      <c r="G5" t="s">
         <v>398</v>
-      </c>
-      <c r="F5" t="s">
-        <v>396</v>
-      </c>
-      <c r="G5" t="s">
-        <v>399</v>
       </c>
       <c r="H5" s="1">
         <v>595</v>
@@ -2531,16 +2531,16 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
+        <v>401</v>
+      </c>
+      <c r="C6" t="s">
+        <v>405</v>
+      </c>
+      <c r="F6" t="s">
+        <v>395</v>
+      </c>
+      <c r="G6" t="s">
         <v>402</v>
-      </c>
-      <c r="C6" t="s">
-        <v>406</v>
-      </c>
-      <c r="F6" t="s">
-        <v>396</v>
-      </c>
-      <c r="G6" t="s">
-        <v>403</v>
       </c>
       <c r="H6" s="1">
         <v>52</v>
@@ -2555,16 +2555,16 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
+        <v>403</v>
+      </c>
+      <c r="C7" t="s">
+        <v>406</v>
+      </c>
+      <c r="F7" t="s">
+        <v>395</v>
+      </c>
+      <c r="G7" t="s">
         <v>404</v>
-      </c>
-      <c r="C7" t="s">
-        <v>407</v>
-      </c>
-      <c r="F7" t="s">
-        <v>396</v>
-      </c>
-      <c r="G7" t="s">
-        <v>405</v>
       </c>
       <c r="H7" s="1">
         <v>67</v>
@@ -2579,13 +2579,13 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
+        <v>407</v>
+      </c>
+      <c r="C8" t="s">
         <v>408</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>409</v>
-      </c>
-      <c r="D8" t="s">
-        <v>410</v>
       </c>
       <c r="E8">
         <v>4970</v>
@@ -2594,7 +2594,7 @@
         <v>44</v>
       </c>
       <c r="G8" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="H8" s="1">
         <v>15.19</v>
@@ -2606,16 +2606,16 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
+        <v>411</v>
+      </c>
+      <c r="D9" t="s">
         <v>412</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>413</v>
       </c>
-      <c r="E9" t="s">
+      <c r="J9" t="s">
         <v>414</v>
-      </c>
-      <c r="J9" t="s">
-        <v>415</v>
       </c>
     </row>
   </sheetData>
@@ -2629,7 +2629,7 @@
   <dimension ref="A2:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2695,7 +2695,7 @@
         <v>350</v>
       </c>
       <c r="C3" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="E3" s="2"/>
       <c r="H3" s="1"/>
@@ -2709,16 +2709,16 @@
         <v>352</v>
       </c>
       <c r="C4" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D4" t="s">
         <v>351</v>
       </c>
       <c r="E4" t="s">
+        <v>355</v>
+      </c>
+      <c r="F4" t="s">
         <v>356</v>
-      </c>
-      <c r="F4" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -2732,10 +2732,10 @@
         <v>354</v>
       </c>
       <c r="E5" t="s">
-        <v>355</v>
+        <v>436</v>
       </c>
       <c r="F5" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -2743,16 +2743,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C6" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D6" t="s">
         <v>15</v>
       </c>
       <c r="E6" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -2760,19 +2760,19 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C7" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D7" t="s">
         <v>15</v>
       </c>
       <c r="E7" t="s">
+        <v>360</v>
+      </c>
+      <c r="F7" t="s">
         <v>361</v>
-      </c>
-      <c r="F7" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -2780,16 +2780,16 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C8" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D8" t="s">
         <v>15</v>
       </c>
       <c r="E8" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -2797,19 +2797,19 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C9" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D9" t="s">
         <v>15</v>
       </c>
       <c r="E9" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F9" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -2817,19 +2817,19 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C10" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D10" t="s">
         <v>15</v>
       </c>
       <c r="E10" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F10" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -2837,16 +2837,16 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C11" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D11" t="s">
         <v>15</v>
       </c>
       <c r="E11" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -2854,19 +2854,19 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C12" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D12" t="s">
         <v>15</v>
       </c>
       <c r="E12" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F12" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -2874,19 +2874,19 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C13" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D13" t="s">
         <v>15</v>
       </c>
       <c r="E13" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F13" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -2894,16 +2894,16 @@
         <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C14" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D14" t="s">
         <v>15</v>
       </c>
       <c r="E14" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -2911,16 +2911,16 @@
         <v>4</v>
       </c>
       <c r="B15" t="s">
+        <v>430</v>
+      </c>
+      <c r="C15" t="s">
+        <v>433</v>
+      </c>
+      <c r="E15" t="s">
         <v>431</v>
       </c>
-      <c r="C15" t="s">
-        <v>434</v>
-      </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>432</v>
-      </c>
-      <c r="F15" t="s">
-        <v>433</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -2928,10 +2928,10 @@
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C16" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="F16" t="s">
         <v>0</v>
@@ -3082,13 +3082,13 @@
         <v>15</v>
       </c>
       <c r="G6" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="H6">
         <v>5.61</v>
       </c>
       <c r="J6" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="K6" t="s">
         <v>287</v>
@@ -3114,13 +3114,13 @@
         <v>15</v>
       </c>
       <c r="G7" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="H7">
         <v>5.61</v>
       </c>
       <c r="J7" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="K7" t="s">
         <v>296</v>
@@ -3143,7 +3143,7 @@
         <v>15</v>
       </c>
       <c r="G8" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="H8">
         <v>20.21</v>
@@ -3924,13 +3924,13 @@
         <v>28</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="G23" t="s">
         <v>194</v>
       </c>
       <c r="H23" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="I23" s="1">
         <v>40</v>
@@ -4831,13 +4831,13 @@
         <v>28</v>
       </c>
       <c r="F26" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="G26" s="3" t="s">
         <v>194</v>
       </c>
       <c r="H26" s="18" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="M26" t="s">
         <v>195</v>

</xml_diff>

<commit_message>
Add mechanical parts to FlySong RGB
</commit_message>
<xml_diff>
--- a/96ChannelRecordingRig.xlsx
+++ b/96ChannelRecordingRig.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sawtelles\Documents\GitHub\FlySong\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5C14766-262E-468C-9701-0C51BE371F16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45C82265-2DBA-409A-B285-0B9F9CFE3B78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="1125" windowWidth="27630" windowHeight="14250" activeTab="2" xr2:uid="{0B008E79-2D1D-4383-A393-19DDE4F60BB8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" activeTab="2" xr2:uid="{0B008E79-2D1D-4383-A393-19DDE4F60BB8}"/>
   </bookViews>
   <sheets>
     <sheet name="Top Level" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="437">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="436">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -1294,9 +1294,6 @@
     <t xml:space="preserve">12" length </t>
   </si>
   <si>
-    <t>Cut corners to fit</t>
-  </si>
-  <si>
     <t>Cut to 7" length</t>
   </si>
   <si>
@@ -1336,15 +1333,9 @@
     <t>Mirror Supports</t>
   </si>
   <si>
-    <t>tiltedReflectorAligner.stl</t>
-  </si>
-  <si>
     <t>3-D print</t>
   </si>
   <si>
-    <t>tiltedReflectorAligner</t>
-  </si>
-  <si>
     <t>RGB Interconnect Cable</t>
   </si>
   <si>
@@ -1352,6 +1343,12 @@
   </si>
   <si>
     <t xml:space="preserve"> 2447 White 1/16" thick</t>
+  </si>
+  <si>
+    <t>Laser Cut using FlySongRGBMirror.dxf</t>
+  </si>
+  <si>
+    <t>TslotMiirrorSupport.stl</t>
   </si>
 </sst>
 </file>
@@ -2276,7 +2273,7 @@
         <v>58</v>
       </c>
       <c r="E19" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="F19" t="s">
         <v>10</v>
@@ -2629,7 +2626,7 @@
   <dimension ref="A2:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2639,7 +2636,7 @@
     <col min="3" max="3" width="92.28515625" customWidth="1"/>
     <col min="4" max="4" width="14.85546875" customWidth="1"/>
     <col min="5" max="5" width="25.140625" customWidth="1"/>
-    <col min="6" max="6" width="29.85546875" customWidth="1"/>
+    <col min="6" max="6" width="38.5703125" customWidth="1"/>
     <col min="7" max="7" width="26.5703125" customWidth="1"/>
     <col min="11" max="11" width="22.5703125" customWidth="1"/>
     <col min="12" max="12" width="26.85546875" customWidth="1"/>
@@ -2695,7 +2692,7 @@
         <v>350</v>
       </c>
       <c r="C3" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="E3" s="2"/>
       <c r="H3" s="1"/>
@@ -2709,7 +2706,7 @@
         <v>352</v>
       </c>
       <c r="C4" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D4" t="s">
         <v>351</v>
@@ -2732,10 +2729,10 @@
         <v>354</v>
       </c>
       <c r="E5" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="F5" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -2746,7 +2743,7 @@
         <v>358</v>
       </c>
       <c r="C6" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D6" t="s">
         <v>15</v>
@@ -2783,7 +2780,7 @@
         <v>362</v>
       </c>
       <c r="C8" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D8" t="s">
         <v>15</v>
@@ -2829,7 +2826,7 @@
         <v>360</v>
       </c>
       <c r="F10" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -2857,7 +2854,7 @@
         <v>369</v>
       </c>
       <c r="C12" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D12" t="s">
         <v>15</v>
@@ -2866,7 +2863,7 @@
         <v>370</v>
       </c>
       <c r="F12" t="s">
-        <v>417</v>
+        <v>434</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -2894,33 +2891,33 @@
         <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C14" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D14" t="s">
         <v>15</v>
       </c>
       <c r="E14" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B15" t="s">
+        <v>429</v>
+      </c>
+      <c r="C15" t="s">
+        <v>0</v>
+      </c>
+      <c r="E15" t="s">
+        <v>435</v>
+      </c>
+      <c r="F15" t="s">
         <v>430</v>
-      </c>
-      <c r="C15" t="s">
-        <v>433</v>
-      </c>
-      <c r="E15" t="s">
-        <v>431</v>
-      </c>
-      <c r="F15" t="s">
-        <v>432</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -2928,10 +2925,10 @@
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="C16" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="F16" t="s">
         <v>0</v>
@@ -3143,7 +3140,7 @@
         <v>15</v>
       </c>
       <c r="G8" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="H8">
         <v>20.21</v>

</xml_diff>

<commit_message>
Update BOMs and boards, add miniFlySong photo
</commit_message>
<xml_diff>
--- a/96ChannelRecordingRig.xlsx
+++ b/96ChannelRecordingRig.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sawtelles\Documents\GitHub\FlySong\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45C82265-2DBA-409A-B285-0B9F9CFE3B78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3191E938-F56B-4013-96DA-F5A03723197F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" activeTab="2" xr2:uid="{0B008E79-2D1D-4383-A393-19DDE4F60BB8}"/>
+    <workbookView xWindow="-75" yWindow="2355" windowWidth="30090" windowHeight="12240" activeTab="5" xr2:uid="{0B008E79-2D1D-4383-A393-19DDE4F60BB8}"/>
   </bookViews>
   <sheets>
     <sheet name="Top Level" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="436">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="443">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -1057,9 +1057,6 @@
     <t xml:space="preserve">C1 C2 C3 C4 C5 C6 C7 C8 </t>
   </si>
   <si>
-    <t>.1 0805</t>
-  </si>
-  <si>
     <t>heat melt to bottom of chamber body</t>
   </si>
   <si>
@@ -1349,6 +1346,30 @@
   </si>
   <si>
     <t>TslotMiirrorSupport.stl</t>
+  </si>
+  <si>
+    <t>TRH100A280-12E13-Level-VI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cincon </t>
+  </si>
+  <si>
+    <t>Desktop AC Adapters, Level VI, Desktop, 100 Watt, 90-264VAC Input, 28VDC Output,</t>
+  </si>
+  <si>
+    <t>Power Supply</t>
+  </si>
+  <si>
+    <t>Multilayer Ceramic Capacitor, 0.1 uF, 50 V, ± 10%, X7R, 0805</t>
+  </si>
+  <si>
+    <t>Samsung</t>
+  </si>
+  <si>
+    <t>CL21B104KBCNNNC</t>
+  </si>
+  <si>
+    <t>1276-1003-1-ND</t>
   </si>
 </sst>
 </file>
@@ -1987,22 +2008,22 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C9" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="F9" t="s">
         <v>15</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="H9" s="1">
         <v>59.62</v>
       </c>
       <c r="J9" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -2010,16 +2031,16 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C10" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="F10" t="s">
         <v>15</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="H10" s="1">
         <v>25.34</v>
@@ -2030,22 +2051,22 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
+        <v>377</v>
+      </c>
+      <c r="C11" t="s">
         <v>378</v>
-      </c>
-      <c r="C11" t="s">
-        <v>379</v>
       </c>
       <c r="F11" t="s">
         <v>15</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="H11" s="1">
         <v>17.239999999999998</v>
       </c>
       <c r="J11" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -2068,7 +2089,7 @@
         <v>15</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="H12" s="1">
         <v>7.71</v>
@@ -2273,7 +2294,7 @@
         <v>58</v>
       </c>
       <c r="E19" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="F19" t="s">
         <v>10</v>
@@ -2303,7 +2324,7 @@
         <v>278</v>
       </c>
       <c r="J20" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -2340,7 +2361,7 @@
         <v>3500</v>
       </c>
       <c r="J22" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -2348,21 +2369,21 @@
         <v>2</v>
       </c>
       <c r="B23" t="s">
+        <v>386</v>
+      </c>
+      <c r="C23" t="s">
         <v>387</v>
-      </c>
-      <c r="C23" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D24" t="s">
         <v>58</v>
       </c>
       <c r="E24" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="I24" s="1">
         <v>0</v>
@@ -2373,13 +2394,13 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D25" t="s">
         <v>28</v>
       </c>
       <c r="E25" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="I25" s="1">
         <v>0</v>
@@ -2387,18 +2408,18 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
+        <v>346</v>
+      </c>
+      <c r="C26" t="s">
         <v>347</v>
       </c>
-      <c r="C26" t="s">
+      <c r="J26" t="s">
         <v>348</v>
-      </c>
-      <c r="J26" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="I28" s="1">
         <f>SUM(I4:I25)</f>
@@ -2433,7 +2454,7 @@
   <sheetData>
     <row r="1" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="H1" s="12"/>
     </row>
@@ -2451,13 +2472,13 @@
         <v>3</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="F3" s="13" t="s">
         <v>5</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="H3" s="12" t="s">
         <v>73</v>
@@ -2474,22 +2495,22 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C4" t="s">
+        <v>390</v>
+      </c>
+      <c r="D4" t="s">
         <v>391</v>
       </c>
-      <c r="D4" t="s">
-        <v>392</v>
-      </c>
       <c r="E4" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="F4" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>395</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>396</v>
       </c>
       <c r="H4" s="1">
         <v>850</v>
@@ -2504,16 +2525,16 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C5" t="s">
+        <v>396</v>
+      </c>
+      <c r="F5" t="s">
+        <v>394</v>
+      </c>
+      <c r="G5" t="s">
         <v>397</v>
-      </c>
-      <c r="F5" t="s">
-        <v>395</v>
-      </c>
-      <c r="G5" t="s">
-        <v>398</v>
       </c>
       <c r="H5" s="1">
         <v>595</v>
@@ -2528,16 +2549,16 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
+        <v>400</v>
+      </c>
+      <c r="C6" t="s">
+        <v>404</v>
+      </c>
+      <c r="F6" t="s">
+        <v>394</v>
+      </c>
+      <c r="G6" t="s">
         <v>401</v>
-      </c>
-      <c r="C6" t="s">
-        <v>405</v>
-      </c>
-      <c r="F6" t="s">
-        <v>395</v>
-      </c>
-      <c r="G6" t="s">
-        <v>402</v>
       </c>
       <c r="H6" s="1">
         <v>52</v>
@@ -2552,16 +2573,16 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
+        <v>402</v>
+      </c>
+      <c r="C7" t="s">
+        <v>405</v>
+      </c>
+      <c r="F7" t="s">
+        <v>394</v>
+      </c>
+      <c r="G7" t="s">
         <v>403</v>
-      </c>
-      <c r="C7" t="s">
-        <v>406</v>
-      </c>
-      <c r="F7" t="s">
-        <v>395</v>
-      </c>
-      <c r="G7" t="s">
-        <v>404</v>
       </c>
       <c r="H7" s="1">
         <v>67</v>
@@ -2576,13 +2597,13 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
+        <v>406</v>
+      </c>
+      <c r="C8" t="s">
         <v>407</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>408</v>
-      </c>
-      <c r="D8" t="s">
-        <v>409</v>
       </c>
       <c r="E8">
         <v>4970</v>
@@ -2591,7 +2612,7 @@
         <v>44</v>
       </c>
       <c r="G8" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="H8" s="1">
         <v>15.19</v>
@@ -2603,16 +2624,16 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
+        <v>410</v>
+      </c>
+      <c r="D9" t="s">
         <v>411</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>412</v>
       </c>
-      <c r="E9" t="s">
+      <c r="J9" t="s">
         <v>413</v>
-      </c>
-      <c r="J9" t="s">
-        <v>414</v>
       </c>
     </row>
   </sheetData>
@@ -2623,10 +2644,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE26C6C8-A75F-4B07-BB7A-B53D3B568C33}">
-  <dimension ref="A2:M16"/>
+  <dimension ref="A2:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2635,7 +2656,7 @@
     <col min="2" max="2" width="23.140625" customWidth="1"/>
     <col min="3" max="3" width="92.28515625" customWidth="1"/>
     <col min="4" max="4" width="14.85546875" customWidth="1"/>
-    <col min="5" max="5" width="25.140625" customWidth="1"/>
+    <col min="5" max="5" width="26.140625" customWidth="1"/>
     <col min="6" max="6" width="38.5703125" customWidth="1"/>
     <col min="7" max="7" width="26.5703125" customWidth="1"/>
     <col min="11" max="11" width="22.5703125" customWidth="1"/>
@@ -2689,10 +2710,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C3" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="E3" s="2"/>
       <c r="H3" s="1"/>
@@ -2703,19 +2724,19 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C4" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D4" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E4" t="s">
+        <v>354</v>
+      </c>
+      <c r="F4" t="s">
         <v>355</v>
-      </c>
-      <c r="F4" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -2723,16 +2744,16 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
+        <v>352</v>
+      </c>
+      <c r="D5" t="s">
         <v>353</v>
       </c>
-      <c r="D5" t="s">
-        <v>354</v>
-      </c>
       <c r="E5" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F5" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -2740,16 +2761,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C6" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D6" t="s">
         <v>15</v>
       </c>
       <c r="E6" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -2757,19 +2778,19 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D7" t="s">
         <v>15</v>
       </c>
       <c r="E7" t="s">
+        <v>359</v>
+      </c>
+      <c r="F7" t="s">
         <v>360</v>
-      </c>
-      <c r="F7" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -2777,16 +2798,16 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C8" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D8" t="s">
         <v>15</v>
       </c>
       <c r="E8" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -2794,19 +2815,19 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C9" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D9" t="s">
         <v>15</v>
       </c>
       <c r="E9" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="F9" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -2814,19 +2835,19 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C10" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D10" t="s">
         <v>15</v>
       </c>
       <c r="E10" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="F10" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -2834,16 +2855,16 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C11" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D11" t="s">
         <v>15</v>
       </c>
       <c r="E11" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -2851,19 +2872,19 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C12" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D12" t="s">
         <v>15</v>
       </c>
       <c r="E12" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F12" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -2871,19 +2892,19 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C13" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D13" t="s">
         <v>15</v>
       </c>
       <c r="E13" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="F13" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -2891,16 +2912,16 @@
         <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C14" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D14" t="s">
         <v>15</v>
       </c>
       <c r="E14" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -2908,16 +2929,16 @@
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C15" t="s">
         <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="F15" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -2925,13 +2946,30 @@
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C16" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F16" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17" t="s">
+        <v>438</v>
+      </c>
+      <c r="C17" t="s">
+        <v>437</v>
+      </c>
+      <c r="D17" t="s">
+        <v>436</v>
+      </c>
+      <c r="E17" t="s">
+        <v>435</v>
       </c>
     </row>
   </sheetData>
@@ -3079,13 +3117,13 @@
         <v>15</v>
       </c>
       <c r="G6" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="H6">
         <v>5.61</v>
       </c>
       <c r="J6" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="K6" t="s">
         <v>287</v>
@@ -3111,13 +3149,13 @@
         <v>15</v>
       </c>
       <c r="G7" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="H7">
         <v>5.61</v>
       </c>
       <c r="J7" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="K7" t="s">
         <v>296</v>
@@ -3140,13 +3178,13 @@
         <v>15</v>
       </c>
       <c r="G8" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="H8">
         <v>20.21</v>
       </c>
       <c r="J8" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
   </sheetData>
@@ -3921,13 +3959,13 @@
         <v>28</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="G23" t="s">
         <v>194</v>
       </c>
       <c r="H23" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="I23" s="1">
         <v>40</v>
@@ -3953,15 +3991,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4EF4737-2343-4468-93BD-3DA932E88D13}">
   <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.140625" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="38.140625" customWidth="1"/>
+    <col min="3" max="3" width="59.85546875" customWidth="1"/>
     <col min="4" max="4" width="45.42578125" customWidth="1"/>
     <col min="5" max="5" width="28.7109375" customWidth="1"/>
     <col min="6" max="6" width="40.85546875" customWidth="1"/>
@@ -4053,7 +4091,7 @@
         <v>0.16</v>
       </c>
       <c r="J4" s="1">
-        <f t="shared" ref="J4:J25" si="0">A4*I4</f>
+        <f t="shared" ref="J4:J27" si="0">A4*I4</f>
         <v>1.28</v>
       </c>
       <c r="L4" t="s">
@@ -4828,13 +4866,17 @@
         <v>28</v>
       </c>
       <c r="F26" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="G26" s="3" t="s">
         <v>194</v>
       </c>
       <c r="H26" s="18" t="s">
-        <v>384</v>
+        <v>383</v>
+      </c>
+      <c r="J26" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="M26" t="s">
         <v>195</v>
@@ -4844,11 +4886,30 @@
       <c r="A27">
         <v>8</v>
       </c>
-      <c r="C27" s="3" t="s">
-        <v>338</v>
+      <c r="C27" t="s">
+        <v>439</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>337</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>440</v>
+      </c>
+      <c r="F27" t="s">
+        <v>441</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="H27" t="s">
+        <v>442</v>
+      </c>
+      <c r="I27" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="J27" s="1">
+        <f t="shared" si="0"/>
+        <v>0.8</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
@@ -4914,7 +4975,7 @@
       <c r="I31" s="1"/>
       <c r="J31" s="1">
         <f>SUM(J4:J30)</f>
-        <v>196.33999999999997</v>
+        <v>197.14</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Backplane BOM, FPGA RGB control error
Backplane BOM had incorrect parts for the BNC and Battery connector
Fixed spelling error in Eagle note
There were errors when the backplane controlled an RGB display via serial control. The serial circular buffer was not being filled correctly at wrap around. Code was changed so that the buffer was filled differently, one value per clock, with one increment of the pointer per clock. This seems to fix the problem.
</commit_message>
<xml_diff>
--- a/96ChannelRecordingRig.xlsx
+++ b/96ChannelRecordingRig.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sawtelles\Documents\GitHub\FlySong\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3191E938-F56B-4013-96DA-F5A03723197F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ED95B7C-EFF1-4443-BFB5-9DBECBF5C6FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-75" yWindow="2355" windowWidth="30090" windowHeight="12240" activeTab="5" xr2:uid="{0B008E79-2D1D-4383-A393-19DDE4F60BB8}"/>
+    <workbookView xWindow="375" yWindow="3450" windowWidth="28800" windowHeight="11295" activeTab="4" xr2:uid="{0B008E79-2D1D-4383-A393-19DDE4F60BB8}"/>
   </bookViews>
   <sheets>
     <sheet name="Top Level" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="443">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="444">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -700,9 +700,6 @@
     <t>J1</t>
   </si>
   <si>
-    <t>36-977-ND</t>
-  </si>
-  <si>
     <t>CONN PWR JACK 2X5.5MM SOLDER</t>
   </si>
   <si>
@@ -727,15 +724,6 @@
     <t>100K</t>
   </si>
   <si>
-    <t>BNCEND_LAUNCH_BNC</t>
-  </si>
-  <si>
-    <t>CONN BNC JACK STR 50OHM EDGE MNT</t>
-  </si>
-  <si>
-    <t>ACX2259-ND</t>
-  </si>
-  <si>
     <t>CON14ST2X7_PLUG</t>
   </si>
   <si>
@@ -829,9 +817,6 @@
     <t>RMCF0805FT49R9CT-ND</t>
   </si>
   <si>
-    <t>Amphenol</t>
-  </si>
-  <si>
     <t>CAP CER 10UF 16V X7R 1210</t>
   </si>
   <si>
@@ -1370,6 +1355,24 @@
   </si>
   <si>
     <t>1276-1003-1-ND</t>
+  </si>
+  <si>
+    <t>5227699-3</t>
+  </si>
+  <si>
+    <t>TE Connectivity AMP Connectors</t>
+  </si>
+  <si>
+    <t>CONN BNC JACK STR 50 OHM PCB</t>
+  </si>
+  <si>
+    <t>BNC</t>
+  </si>
+  <si>
+    <t>A32249-ND</t>
+  </si>
+  <si>
+    <t>36-975-ND</t>
   </si>
 </sst>
 </file>
@@ -1805,8 +1808,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView topLeftCell="C3" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="42.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1873,13 +1876,13 @@
         <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="F4" t="s">
         <v>10</v>
@@ -2008,22 +2011,22 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="C9" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="F9" t="s">
         <v>15</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="H9" s="1">
         <v>59.62</v>
       </c>
       <c r="J9" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -2031,16 +2034,16 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="C10" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="F10" t="s">
         <v>15</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="H10" s="1">
         <v>25.34</v>
@@ -2051,22 +2054,22 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="C11" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="F11" t="s">
         <v>15</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="H11" s="1">
         <v>17.239999999999998</v>
       </c>
       <c r="J11" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -2089,7 +2092,7 @@
         <v>15</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="H12" s="1">
         <v>7.71</v>
@@ -2255,22 +2258,22 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="C18" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="D18" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="E18" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="F18" t="s">
         <v>44</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="H18" s="1">
         <v>8.3800000000000008</v>
@@ -2294,7 +2297,7 @@
         <v>58</v>
       </c>
       <c r="E19" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="F19" t="s">
         <v>10</v>
@@ -2318,13 +2321,13 @@
         <v>3</v>
       </c>
       <c r="B20" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C20" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="J20" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -2335,7 +2338,7 @@
         <v>203</v>
       </c>
       <c r="C21" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="E21" t="s">
         <v>63</v>
@@ -2352,7 +2355,7 @@
         <v>67</v>
       </c>
       <c r="C22" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="E22" t="s">
         <v>193</v>
@@ -2361,7 +2364,7 @@
         <v>3500</v>
       </c>
       <c r="J22" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -2369,21 +2372,21 @@
         <v>2</v>
       </c>
       <c r="B23" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="C23" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="D24" t="s">
         <v>58</v>
       </c>
       <c r="E24" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="I24" s="1">
         <v>0</v>
@@ -2394,13 +2397,13 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="D25" t="s">
         <v>28</v>
       </c>
       <c r="E25" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="I25" s="1">
         <v>0</v>
@@ -2408,18 +2411,18 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="C26" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="J26" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="I28" s="1">
         <f>SUM(I4:I25)</f>
@@ -2454,13 +2457,13 @@
   <sheetData>
     <row r="1" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="H1" s="12"/>
     </row>
     <row r="3" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>69</v>
@@ -2472,13 +2475,13 @@
         <v>3</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="F3" s="13" t="s">
         <v>5</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="H3" s="12" t="s">
         <v>73</v>
@@ -2495,22 +2498,22 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="C4" t="s">
+        <v>385</v>
+      </c>
+      <c r="D4" t="s">
+        <v>386</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>390</v>
-      </c>
-      <c r="D4" t="s">
-        <v>391</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>389</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>394</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>395</v>
       </c>
       <c r="H4" s="1">
         <v>850</v>
@@ -2525,16 +2528,16 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="C5" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="F5" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="G5" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="H5" s="1">
         <v>595</v>
@@ -2549,16 +2552,16 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="C6" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="F6" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="G6" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="H6" s="1">
         <v>52</v>
@@ -2573,16 +2576,16 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="C7" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="F7" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="G7" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="H7" s="1">
         <v>67</v>
@@ -2597,13 +2600,13 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="C8" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="D8" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="E8">
         <v>4970</v>
@@ -2612,7 +2615,7 @@
         <v>44</v>
       </c>
       <c r="G8" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="H8" s="1">
         <v>15.19</v>
@@ -2624,16 +2627,16 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="D9" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="E9" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="J9" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
     </row>
   </sheetData>
@@ -2666,7 +2669,7 @@
   <sheetData>
     <row r="2" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="B2" s="13" t="s">
         <v>69</v>
@@ -2678,7 +2681,7 @@
         <v>3</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="F2" s="10" t="s">
         <v>17</v>
@@ -2699,10 +2702,10 @@
         <v>76</v>
       </c>
       <c r="L2" s="10" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="M2" s="10" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -2710,10 +2713,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="C3" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="E3" s="2"/>
       <c r="H3" s="1"/>
@@ -2724,19 +2727,19 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="C4" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="D4" t="s">
+        <v>345</v>
+      </c>
+      <c r="E4" t="s">
+        <v>349</v>
+      </c>
+      <c r="F4" t="s">
         <v>350</v>
-      </c>
-      <c r="E4" t="s">
-        <v>354</v>
-      </c>
-      <c r="F4" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -2744,16 +2747,16 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="D5" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="E5" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="F5" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -2761,16 +2764,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="C6" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="D6" t="s">
         <v>15</v>
       </c>
       <c r="E6" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -2778,19 +2781,19 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="C7" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="D7" t="s">
         <v>15</v>
       </c>
       <c r="E7" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="F7" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -2798,16 +2801,16 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="C8" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="D8" t="s">
         <v>15</v>
       </c>
       <c r="E8" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -2815,19 +2818,19 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="C9" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="D9" t="s">
         <v>15</v>
       </c>
       <c r="E9" t="s">
+        <v>354</v>
+      </c>
+      <c r="F9" t="s">
         <v>359</v>
-      </c>
-      <c r="F9" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -2835,19 +2838,19 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="C10" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="D10" t="s">
         <v>15</v>
       </c>
       <c r="E10" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="F10" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -2855,16 +2858,16 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="C11" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="D11" t="s">
         <v>15</v>
       </c>
       <c r="E11" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -2872,19 +2875,19 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="C12" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="D12" t="s">
         <v>15</v>
       </c>
       <c r="E12" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="F12" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -2892,19 +2895,19 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="C13" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="D13" t="s">
         <v>15</v>
       </c>
       <c r="E13" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="F13" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -2912,16 +2915,16 @@
         <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="C14" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="D14" t="s">
         <v>15</v>
       </c>
       <c r="E14" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -2929,16 +2932,16 @@
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="C15" t="s">
         <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="F15" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -2946,10 +2949,10 @@
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="C16" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="F16" t="s">
         <v>0</v>
@@ -2960,16 +2963,16 @@
         <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="C17" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="D17" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="E17" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
     </row>
   </sheetData>
@@ -3001,7 +3004,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -3036,7 +3039,7 @@
         <v>17</v>
       </c>
       <c r="K3" s="10" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -3044,16 +3047,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="C4" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="D4" t="s">
         <v>28</v>
       </c>
       <c r="E4" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="F4" t="s">
         <v>0</v>
@@ -3068,10 +3071,10 @@
         <v>0</v>
       </c>
       <c r="J4" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="K4" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -3079,22 +3082,22 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="C5" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="D5" t="s">
         <v>28</v>
       </c>
       <c r="E5" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="J5" t="s">
+        <v>275</v>
+      </c>
+      <c r="K5" t="s">
         <v>280</v>
-      </c>
-      <c r="K5" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -3102,31 +3105,31 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="C6" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="D6" t="s">
         <v>28</v>
       </c>
       <c r="E6" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="F6" t="s">
         <v>15</v>
       </c>
       <c r="G6" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="H6">
         <v>5.61</v>
       </c>
       <c r="J6" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="K6" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -3134,31 +3137,31 @@
         <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="C7" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="D7" t="s">
         <v>28</v>
       </c>
       <c r="E7" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="F7" t="s">
         <v>15</v>
       </c>
       <c r="G7" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="H7">
         <v>5.61</v>
       </c>
       <c r="J7" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="K7" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -3166,10 +3169,10 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="C8" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="E8" t="s">
         <v>0</v>
@@ -3178,13 +3181,13 @@
         <v>15</v>
       </c>
       <c r="G8" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="H8">
         <v>20.21</v>
       </c>
       <c r="J8" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
     </row>
   </sheetData>
@@ -3197,8 +3200,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:N25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3228,7 +3231,7 @@
     </row>
     <row r="3" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>69</v>
@@ -3243,13 +3246,13 @@
         <v>3</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="G3" s="10" t="s">
         <v>72</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="I3" s="12" t="s">
         <v>73</v>
@@ -3264,10 +3267,10 @@
         <v>76</v>
       </c>
       <c r="M3" s="10" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="N3" s="10" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -3317,20 +3320,20 @@
         <v>41</v>
       </c>
       <c r="F5" s="2">
-        <v>977</v>
+        <v>975</v>
       </c>
       <c r="G5" t="s">
         <v>44</v>
       </c>
       <c r="H5" t="s">
-        <v>219</v>
+        <v>443</v>
       </c>
       <c r="I5" s="1">
-        <v>1.22</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="J5" s="1">
         <f t="shared" ref="J5:J23" si="0">A5*I5</f>
-        <v>1.22</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="L5" t="s">
         <v>78</v>
@@ -3341,16 +3344,16 @@
         <v>1</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="C6" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="D6" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="E6" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="F6" s="2">
         <v>61300411121</v>
@@ -3359,7 +3362,7 @@
         <v>44</v>
       </c>
       <c r="H6" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="I6" s="1">
         <v>0.18</v>
@@ -3377,22 +3380,22 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D7" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="E7" t="s">
         <v>162</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G7" t="s">
         <v>44</v>
       </c>
       <c r="H7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I7" s="1">
         <v>1.44</v>
@@ -3416,7 +3419,7 @@
         <v>84</v>
       </c>
       <c r="D8" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>86</v>
@@ -3446,25 +3449,25 @@
         <v>2</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="C9" t="s">
         <v>223</v>
       </c>
-      <c r="C9" t="s">
-        <v>224</v>
-      </c>
       <c r="D9" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="E9" t="s">
         <v>144</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G9" t="s">
         <v>44</v>
       </c>
       <c r="H9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I9" s="1">
         <v>0.72</v>
@@ -3485,22 +3488,22 @@
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="D10" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="E10" t="s">
         <v>86</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="G10" t="s">
         <v>44</v>
       </c>
       <c r="H10" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="I10" s="1">
         <v>0.65</v>
@@ -3521,22 +3524,22 @@
         <v>49.9</v>
       </c>
       <c r="C11" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="D11" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="E11" t="s">
         <v>184</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="G11" t="s">
         <v>44</v>
       </c>
       <c r="H11" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="I11" s="1">
         <v>0.1</v>
@@ -3554,25 +3557,25 @@
         <v>3</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="C12" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="D12" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="E12" t="s">
         <v>144</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="G12" t="s">
         <v>44</v>
       </c>
       <c r="H12" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="I12" s="1">
         <v>0.36</v>
@@ -3593,22 +3596,22 @@
         <v>191</v>
       </c>
       <c r="C13" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="D13" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="E13" t="s">
         <v>184</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="G13" t="s">
         <v>44</v>
       </c>
       <c r="H13" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="I13" s="1">
         <v>0.1</v>
@@ -3626,25 +3629,25 @@
         <v>1</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="C14" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="D14" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="E14" t="s">
         <v>184</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="G14" t="s">
         <v>44</v>
       </c>
       <c r="H14" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="I14" s="1">
         <v>0.1</v>
@@ -3662,25 +3665,25 @@
         <v>1</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C15" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="D15" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="E15" t="s">
         <v>184</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="G15" t="s">
         <v>44</v>
       </c>
       <c r="H15" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="I15" s="1">
         <v>0.1</v>
@@ -3698,32 +3701,32 @@
         <v>4</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>228</v>
+        <v>441</v>
       </c>
       <c r="C16" t="s">
-        <v>229</v>
+        <v>440</v>
       </c>
       <c r="D16" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="E16" t="s">
-        <v>262</v>
-      </c>
-      <c r="F16" s="2">
-        <v>112640</v>
+        <v>439</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>438</v>
       </c>
       <c r="G16" t="s">
         <v>44</v>
       </c>
       <c r="H16" t="s">
-        <v>230</v>
+        <v>442</v>
       </c>
       <c r="I16" s="1">
-        <v>5.54</v>
+        <v>4.7699999999999996</v>
       </c>
       <c r="J16" s="1">
         <f t="shared" si="0"/>
-        <v>22.16</v>
+        <v>19.079999999999998</v>
       </c>
       <c r="L16" t="s">
         <v>78</v>
@@ -3734,25 +3737,25 @@
         <v>12</v>
       </c>
       <c r="B17" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="C17" t="s">
+        <v>228</v>
+      </c>
+      <c r="D17" t="s">
+        <v>229</v>
+      </c>
+      <c r="E17" t="s">
+        <v>230</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>231</v>
-      </c>
-      <c r="C17" t="s">
-        <v>232</v>
-      </c>
-      <c r="D17" t="s">
-        <v>233</v>
-      </c>
-      <c r="E17" t="s">
-        <v>234</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>235</v>
       </c>
       <c r="G17" t="s">
         <v>44</v>
       </c>
       <c r="H17" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="I17" s="1">
         <v>0.91</v>
@@ -3770,25 +3773,25 @@
         <v>1</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="C18" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D18" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="E18" t="s">
         <v>144</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="G18" t="s">
         <v>44</v>
       </c>
       <c r="H18" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="I18" s="1">
         <v>1.28</v>
@@ -3806,25 +3809,25 @@
         <v>1</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C19" t="s">
+        <v>237</v>
+      </c>
+      <c r="D19" t="s">
+        <v>238</v>
+      </c>
+      <c r="E19" t="s">
+        <v>239</v>
+      </c>
+      <c r="F19" s="2" t="s">
         <v>240</v>
-      </c>
-      <c r="C19" t="s">
-        <v>241</v>
-      </c>
-      <c r="D19" t="s">
-        <v>242</v>
-      </c>
-      <c r="E19" t="s">
-        <v>243</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>244</v>
       </c>
       <c r="G19" t="s">
         <v>44</v>
       </c>
       <c r="H19" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="I19" s="1">
         <v>5.4</v>
@@ -3842,25 +3845,25 @@
         <v>2</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="C20" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="D20" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="E20" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="G20" t="s">
         <v>44</v>
       </c>
       <c r="H20" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="I20" s="1">
         <v>2.1800000000000002</v>
@@ -3878,25 +3881,25 @@
         <v>2</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="C21" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="D21" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="E21" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="G21" t="s">
         <v>44</v>
       </c>
       <c r="H21" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="I21" s="1">
         <v>2.64</v>
@@ -3914,25 +3917,25 @@
         <v>1</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="C22" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="D22" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="E22" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="G22" t="s">
         <v>44</v>
       </c>
       <c r="H22" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="I22" s="1">
         <v>1.26</v>
@@ -3950,7 +3953,7 @@
         <v>1</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>192</v>
@@ -3959,13 +3962,13 @@
         <v>28</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="G23" t="s">
         <v>194</v>
       </c>
       <c r="H23" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="I23" s="1">
         <v>40</v>
@@ -3978,7 +3981,7 @@
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J25" s="1">
         <f>SUM(J4:J24)</f>
-        <v>102.67</v>
+        <v>99.49</v>
       </c>
     </row>
   </sheetData>
@@ -3991,7 +3994,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4EF4737-2343-4468-93BD-3DA932E88D13}">
   <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+    <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
@@ -4020,7 +4023,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>69</v>
@@ -4035,13 +4038,13 @@
         <v>3</v>
       </c>
       <c r="F3" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="G3" t="s">
         <v>72</v>
       </c>
       <c r="H3" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>73</v>
@@ -4056,10 +4059,10 @@
         <v>76</v>
       </c>
       <c r="M3" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="N3" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -4181,7 +4184,7 @@
         <v>84</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>94</v>
@@ -4201,7 +4204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>8</v>
       </c>
@@ -4248,7 +4251,7 @@
         <v>100</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>86</v>
@@ -4284,7 +4287,7 @@
         <v>103</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>104</v>
@@ -4866,13 +4869,13 @@
         <v>28</v>
       </c>
       <c r="F26" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="G26" s="3" t="s">
         <v>194</v>
       </c>
       <c r="H26" s="18" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="J26" s="1">
         <f t="shared" si="0"/>
@@ -4887,22 +4890,22 @@
         <v>8</v>
       </c>
       <c r="C27" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="F27" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="G27" s="3" t="s">
         <v>77</v>
       </c>
       <c r="H27" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="I27" s="1">
         <v>0.1</v>

</xml_diff>

<commit_message>
Update BOM, add 3D pdf of rig, add load cover laser cut file fro 12x12 sheet
</commit_message>
<xml_diff>
--- a/96ChannelRecordingRig.xlsx
+++ b/96ChannelRecordingRig.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sawtelles\Documents\GitHub\FlySong\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C6E9214-1B55-4C7D-BA92-E4A6F8ABAD61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D315ECBE-0D4A-4043-95E0-3C292D755ABD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" activeTab="2" xr2:uid="{0B008E79-2D1D-4383-A393-19DDE4F60BB8}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="18240" windowHeight="28320" xr2:uid="{0B008E79-2D1D-4383-A393-19DDE4F60BB8}"/>
   </bookViews>
   <sheets>
     <sheet name="Top Level" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="464">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="467">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -100,9 +100,6 @@
     <t>pkg of 25 - need 4</t>
   </si>
   <si>
-    <t>1 pack</t>
-  </si>
-  <si>
     <t>backplane to breadboard bracket</t>
   </si>
   <si>
@@ -118,9 +115,6 @@
     <t>Nylon Hex Nut, 1/4"-20 Thread Size</t>
   </si>
   <si>
-    <t xml:space="preserve">1 pack </t>
-  </si>
-  <si>
     <t>pkg of 100 need 4</t>
   </si>
   <si>
@@ -139,9 +133,6 @@
     <t>Laser cut from 1/8" acrylic</t>
   </si>
   <si>
-    <t>1 set</t>
-  </si>
-  <si>
     <t>Fasteners for nylon screws</t>
   </si>
   <si>
@@ -1366,9 +1357,6 @@
     <t>Camera Post</t>
   </si>
   <si>
-    <t>47065T679</t>
-  </si>
-  <si>
     <t>Cut to 28" length</t>
   </si>
   <si>
@@ -1420,9 +1408,6 @@
     <t>Black Corner Bracket, 1" Long, for 1" High Rail T-Slotted Framing</t>
   </si>
   <si>
-    <t>47065T237</t>
-  </si>
-  <si>
     <t>T-Slotted Framing, Black Corner Bracket, 1" Long for 2" High Double/Quad Rail</t>
   </si>
   <si>
@@ -1432,7 +1417,31 @@
     <t>2x2 Brackets</t>
   </si>
   <si>
-    <t>Raer Mirror Supports</t>
+    <t>$ea</t>
+  </si>
+  <si>
+    <t>$ total</t>
+  </si>
+  <si>
+    <t>7x7 controller</t>
+  </si>
+  <si>
+    <t>TOTAL length needed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOTAL </t>
+  </si>
+  <si>
+    <t>47065T474</t>
+  </si>
+  <si>
+    <t>47065T695</t>
+  </si>
+  <si>
+    <t>Rear Mirror Supports</t>
+  </si>
+  <si>
+    <t>3-D printed</t>
   </si>
 </sst>
 </file>
@@ -1510,7 +1519,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1552,6 +1561,15 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1871,8 +1889,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView topLeftCell="C3" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+    <sheetView tabSelected="1" topLeftCell="E3" workbookViewId="0">
+      <selection activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="42.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1890,10 +1908,10 @@
   <sheetData>
     <row r="1" spans="1:10" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G1" s="16"/>
       <c r="H1" s="17"/>
@@ -1904,7 +1922,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>2</v>
@@ -1939,13 +1957,13 @@
         <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="F4" t="s">
         <v>10</v>
@@ -1966,7 +1984,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
@@ -1987,33 +2005,37 @@
         <v>27.04</v>
       </c>
       <c r="I5" s="1">
-        <f t="shared" ref="I5:I16" si="0">A5*H5</f>
+        <f t="shared" ref="I5:I27" si="0">A5*H5</f>
         <v>108.16</v>
       </c>
       <c r="J5" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="D6" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>448</v>
+        <v>444</v>
+      </c>
+      <c r="I6" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="J6" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>19</v>
+      <c r="A7">
+        <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
         <v>14</v>
@@ -2028,6 +2050,7 @@
         <v>8.0500000000000007</v>
       </c>
       <c r="I7" s="1">
+        <f t="shared" si="0"/>
         <v>8.0500000000000007</v>
       </c>
       <c r="J7" t="s">
@@ -2035,55 +2058,57 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>19</v>
+      <c r="A8">
+        <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="F8" t="s">
         <v>15</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H8" s="1">
         <v>9.57</v>
       </c>
       <c r="I8" s="1">
+        <f t="shared" si="0"/>
         <v>9.57</v>
       </c>
       <c r="J8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" t="s">
-        <v>24</v>
       </c>
       <c r="F9" t="s">
         <v>15</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="H9" s="1">
         <v>9.65</v>
       </c>
       <c r="I9" s="1">
-        <v>9.75</v>
+        <f t="shared" si="0"/>
+        <v>9.65</v>
       </c>
       <c r="J9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -2091,22 +2116,26 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="C10" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="F10" t="s">
         <v>15</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="H10" s="1">
         <v>59.62</v>
       </c>
+      <c r="I10" s="1">
+        <f t="shared" si="0"/>
+        <v>59.62</v>
+      </c>
       <c r="J10" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -2114,19 +2143,23 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="C11" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="F11" t="s">
         <v>15</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="H11" s="1">
         <v>25.34</v>
+      </c>
+      <c r="I11" s="1">
+        <f t="shared" si="0"/>
+        <v>50.68</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -2134,54 +2167,59 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="C12" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="F12" t="s">
         <v>15</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="H12" s="1">
         <v>17.239999999999998</v>
       </c>
+      <c r="I12" s="1">
+        <f t="shared" si="0"/>
+        <v>17.239999999999998</v>
+      </c>
       <c r="J12" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>32</v>
+      <c r="A13">
+        <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D13" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F13" t="s">
         <v>15</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="H13" s="1">
         <v>7.71</v>
       </c>
       <c r="I13" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>7.71</v>
       </c>
       <c r="J13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -2189,25 +2227,26 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C14" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E14" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="H14" s="1">
         <v>0</v>
       </c>
       <c r="I14" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -2215,22 +2254,22 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" t="s">
         <v>37</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15" t="s">
+        <v>41</v>
+      </c>
+      <c r="G15" s="9" t="s">
         <v>40</v>
-      </c>
-      <c r="D15" t="s">
-        <v>41</v>
-      </c>
-      <c r="E15" t="s">
-        <v>42</v>
-      </c>
-      <c r="F15" t="s">
-        <v>44</v>
-      </c>
-      <c r="G15" s="9" t="s">
-        <v>43</v>
       </c>
       <c r="H15" s="1">
         <v>2.2000000000000002</v>
@@ -2245,22 +2284,22 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C16" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D16" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E16" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F16" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="H16" s="1">
         <v>18.46</v>
@@ -2275,32 +2314,32 @@
         <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" t="s">
         <v>50</v>
       </c>
-      <c r="D17" t="s">
-        <v>51</v>
-      </c>
-      <c r="E17" t="s">
-        <v>53</v>
-      </c>
       <c r="F17" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H17" s="1">
         <v>3.98</v>
       </c>
       <c r="I17" s="1">
-        <f>A17*H17</f>
+        <f t="shared" si="0"/>
         <v>31.84</v>
       </c>
       <c r="J17" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -2308,16 +2347,16 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" t="s">
         <v>55</v>
       </c>
-      <c r="C18" t="s">
-        <v>57</v>
-      </c>
-      <c r="D18" t="s">
-        <v>58</v>
-      </c>
       <c r="E18" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F18" t="s">
         <v>10</v>
@@ -2329,7 +2368,7 @@
         <v>199.95</v>
       </c>
       <c r="I18" s="1">
-        <f>A18*H18</f>
+        <f t="shared" si="0"/>
         <v>199.95</v>
       </c>
     </row>
@@ -2338,28 +2377,28 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C19" t="s">
+        <v>292</v>
+      </c>
+      <c r="D19" t="s">
+        <v>293</v>
+      </c>
+      <c r="E19" t="s">
+        <v>294</v>
+      </c>
+      <c r="F19" t="s">
+        <v>41</v>
+      </c>
+      <c r="G19" s="9" t="s">
         <v>295</v>
-      </c>
-      <c r="D19" t="s">
-        <v>296</v>
-      </c>
-      <c r="E19" t="s">
-        <v>297</v>
-      </c>
-      <c r="F19" t="s">
-        <v>44</v>
-      </c>
-      <c r="G19" s="9" t="s">
-        <v>298</v>
       </c>
       <c r="H19" s="1">
         <v>8.3800000000000008</v>
       </c>
       <c r="I19" s="1">
-        <f>A19*H19</f>
+        <f t="shared" si="0"/>
         <v>8.3800000000000008</v>
       </c>
     </row>
@@ -2368,16 +2407,16 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C20" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D20" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E20" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="F20" t="s">
         <v>10</v>
@@ -2389,11 +2428,11 @@
         <v>10</v>
       </c>
       <c r="I20" s="1">
-        <f>A20*H20</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="J20" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -2401,13 +2440,17 @@
         <v>3</v>
       </c>
       <c r="B21" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="C21" t="s">
-        <v>273</v>
+        <v>270</v>
+      </c>
+      <c r="I21" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="J21" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -2415,16 +2458,21 @@
         <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C22" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="E22" t="s">
-        <v>63</v>
+        <v>60</v>
+      </c>
+      <c r="H22" s="1">
+        <f>'Backplane Assembly'!$J$25</f>
+        <v>99.49</v>
       </c>
       <c r="I22" s="1">
-        <v>100</v>
+        <f t="shared" si="0"/>
+        <v>99.49</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -2432,19 +2480,24 @@
         <v>12</v>
       </c>
       <c r="B23" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C23" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="E23" t="s">
-        <v>193</v>
+        <v>190</v>
+      </c>
+      <c r="H23" s="1">
+        <f>'Microphone Assembly'!$J$31</f>
+        <v>212.14</v>
       </c>
       <c r="I23" s="1">
-        <v>3500</v>
+        <f t="shared" si="0"/>
+        <v>2545.6799999999998</v>
       </c>
       <c r="J23" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -2452,23 +2505,32 @@
         <v>2</v>
       </c>
       <c r="B24" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="C24" t="s">
-        <v>376</v>
+        <v>373</v>
+      </c>
+      <c r="H24" s="1">
+        <f>'Camera Assembly'!$I$11</f>
+        <v>3158.38</v>
+      </c>
+      <c r="I24" s="1">
+        <f t="shared" si="0"/>
+        <v>6316.76</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="D25" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E25" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="I25" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J25" t="s">
@@ -2477,36 +2539,48 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="D26" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E26" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="I26" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>1</v>
+      </c>
       <c r="B27" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="C27" t="s">
-        <v>342</v>
+        <v>339</v>
+      </c>
+      <c r="H27" s="1">
+        <f>'RGB-IR Lighting'!$I$30</f>
+        <v>1920.6419999999998</v>
+      </c>
+      <c r="I27" s="1">
+        <f t="shared" si="0"/>
+        <v>1920.6419999999998</v>
       </c>
       <c r="J27" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="I29" s="1">
-        <f>SUM(I4:I26)</f>
-        <v>4194.3599999999997</v>
+        <f>SUM(I4:I27)</f>
+        <v>11612.082</v>
       </c>
     </row>
   </sheetData>
@@ -2517,10 +2591,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04FA5B49-A75E-4EE7-920B-8ED9DAF93836}">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2537,37 +2611,37 @@
   <sheetData>
     <row r="1" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="H1" s="12"/>
     </row>
     <row r="3" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>3</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="F3" s="13" t="s">
         <v>5</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="H3" s="12" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="J3" s="10" t="s">
         <v>17</v>
@@ -2578,22 +2652,22 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="C4" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="D4" t="s">
+        <v>377</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>380</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>378</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>383</v>
-      </c>
       <c r="G4" s="2" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="H4" s="1">
         <v>850</v>
@@ -2608,16 +2682,16 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="C5" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="F5" t="s">
+        <v>380</v>
+      </c>
+      <c r="G5" t="s">
         <v>383</v>
-      </c>
-      <c r="G5" t="s">
-        <v>386</v>
       </c>
       <c r="H5" s="1">
         <v>595</v>
@@ -2632,16 +2706,16 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="C6" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="F6" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="G6" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="H6" s="1">
         <v>52</v>
@@ -2656,16 +2730,16 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
+        <v>388</v>
+      </c>
+      <c r="C7" t="s">
         <v>391</v>
       </c>
-      <c r="C7" t="s">
-        <v>394</v>
-      </c>
       <c r="F7" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="G7" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="H7" s="1">
         <v>67</v>
@@ -2680,22 +2754,22 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="C8" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="D8" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="E8">
         <v>4970</v>
       </c>
       <c r="F8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G8" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="H8" s="1">
         <v>15.19</v>
@@ -2707,16 +2781,25 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
+        <v>396</v>
+      </c>
+      <c r="D9" t="s">
+        <v>397</v>
+      </c>
+      <c r="E9" t="s">
+        <v>398</v>
+      </c>
+      <c r="J9" t="s">
         <v>399</v>
       </c>
-      <c r="D9" t="s">
-        <v>400</v>
-      </c>
-      <c r="E9" t="s">
-        <v>401</v>
-      </c>
-      <c r="J9" t="s">
-        <v>402</v>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>335</v>
+      </c>
+      <c r="I11" s="1">
+        <f>SUM(I4:I9)</f>
+        <v>3158.38</v>
       </c>
     </row>
   </sheetData>
@@ -2727,519 +2810,722 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE26C6C8-A75F-4B07-BB7A-B53D3B568C33}">
-  <dimension ref="A1:P23"/>
+  <dimension ref="A1:T30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
     <col min="2" max="2" width="23.140625" customWidth="1"/>
-    <col min="3" max="3" width="92.28515625" customWidth="1"/>
+    <col min="3" max="3" width="65.42578125" customWidth="1"/>
     <col min="4" max="4" width="14.85546875" customWidth="1"/>
     <col min="5" max="5" width="26.140625" customWidth="1"/>
-    <col min="6" max="6" width="35.140625" customWidth="1"/>
-    <col min="7" max="7" width="7.5703125" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" customWidth="1"/>
-    <col min="9" max="9" width="7" customWidth="1"/>
-    <col min="10" max="10" width="11.5703125" customWidth="1"/>
-    <col min="14" max="14" width="22.5703125" customWidth="1"/>
-    <col min="15" max="15" width="26.85546875" customWidth="1"/>
-    <col min="16" max="16" width="22.42578125" customWidth="1"/>
+    <col min="6" max="6" width="4.85546875" customWidth="1"/>
+    <col min="7" max="7" width="5.28515625" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" customWidth="1"/>
+    <col min="10" max="10" width="35.140625" customWidth="1"/>
+    <col min="11" max="11" width="7.5703125" customWidth="1"/>
+    <col min="12" max="12" width="13.5703125" customWidth="1"/>
+    <col min="13" max="13" width="7" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" customWidth="1"/>
+    <col min="18" max="18" width="22.5703125" customWidth="1"/>
+    <col min="19" max="19" width="26.85546875" customWidth="1"/>
+    <col min="20" max="20" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="G1" s="19" t="s">
-        <v>451</v>
-      </c>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19" t="s">
-        <v>452</v>
-      </c>
-      <c r="J1" s="19"/>
-    </row>
-    <row r="2" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="K1" s="19" t="s">
+        <v>447</v>
+      </c>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19" t="s">
+        <v>448</v>
+      </c>
+      <c r="N1" s="19"/>
+    </row>
+    <row r="2" spans="1:20" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>3</v>
       </c>
       <c r="E2" s="13" t="s">
+        <v>241</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>378</v>
+      </c>
+      <c r="H2" s="21" t="s">
+        <v>458</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>459</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>449</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>450</v>
+      </c>
+      <c r="M2" s="10" t="s">
+        <v>449</v>
+      </c>
+      <c r="N2" s="10" t="s">
+        <v>450</v>
+      </c>
+      <c r="O2" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="P2" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q2" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="R2" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="S2" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="T2" s="10" t="s">
         <v>244</v>
       </c>
-      <c r="F2" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>453</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>454</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>453</v>
-      </c>
-      <c r="J2" s="10" t="s">
-        <v>454</v>
-      </c>
-      <c r="K2" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="L2" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="M2" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="N2" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="O2" s="10" t="s">
-        <v>246</v>
-      </c>
-      <c r="P2" s="10" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="C3" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="E3" s="2"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="20">
+        <v>298.75599999999997</v>
+      </c>
+      <c r="I3" s="22">
+        <f>H3*A3</f>
+        <v>597.51199999999994</v>
+      </c>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
-        <v>346</v>
-      </c>
-      <c r="C4" t="s">
-        <v>411</v>
-      </c>
-      <c r="D4" t="s">
-        <v>345</v>
-      </c>
-      <c r="E4" t="s">
-        <v>349</v>
-      </c>
-      <c r="F4" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>460</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="20">
+        <v>90.11</v>
+      </c>
+      <c r="I4" s="22">
+        <f t="shared" ref="I4:I26" si="0">H4*A4</f>
+        <v>180.22</v>
+      </c>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
       <c r="B5" t="s">
+        <v>343</v>
+      </c>
+      <c r="C5" t="s">
+        <v>408</v>
+      </c>
+      <c r="D5" t="s">
+        <v>342</v>
+      </c>
+      <c r="E5" t="s">
+        <v>346</v>
+      </c>
+      <c r="H5" s="1">
+        <v>172.4</v>
+      </c>
+      <c r="I5" s="22">
+        <f t="shared" si="0"/>
+        <v>344.8</v>
+      </c>
+      <c r="J5" t="s">
         <v>347</v>
       </c>
-      <c r="D5" t="s">
-        <v>348</v>
-      </c>
-      <c r="E5" t="s">
-        <v>418</v>
-      </c>
-      <c r="F5" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>344</v>
+      </c>
+      <c r="D6" t="s">
+        <v>345</v>
+      </c>
+      <c r="E6" t="s">
+        <v>415</v>
+      </c>
+      <c r="I6" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J6" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
-        <v>352</v>
-      </c>
-      <c r="C6" t="s">
-        <v>409</v>
-      </c>
-      <c r="D6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>2</v>
-      </c>
       <c r="B7" t="s">
-        <v>436</v>
+        <v>349</v>
       </c>
       <c r="C7" t="s">
-        <v>367</v>
+        <v>406</v>
       </c>
       <c r="D7" t="s">
         <v>15</v>
       </c>
       <c r="E7" t="s">
-        <v>353</v>
-      </c>
-      <c r="F7" t="s">
-        <v>435</v>
-      </c>
-      <c r="I7">
-        <v>4.5</v>
-      </c>
-      <c r="J7">
-        <f>A7*I7</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+      <c r="H7" s="1">
+        <v>49.83</v>
+      </c>
+      <c r="I7" s="22">
+        <f t="shared" si="0"/>
+        <v>199.32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="C8" t="s">
-        <v>438</v>
+        <v>364</v>
       </c>
       <c r="D8" t="s">
         <v>15</v>
       </c>
       <c r="E8" t="s">
-        <v>363</v>
-      </c>
-      <c r="F8" t="s">
+        <v>350</v>
+      </c>
+      <c r="I8" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J8" t="s">
+        <v>432</v>
+      </c>
+      <c r="M8">
+        <v>4.5</v>
+      </c>
+      <c r="N8">
+        <f>A8*M8</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>434</v>
+      </c>
+      <c r="C9" t="s">
         <v>435</v>
-      </c>
-      <c r="G8">
-        <v>4.5</v>
-      </c>
-      <c r="H8">
-        <f>A8*G8</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>3</v>
-      </c>
-      <c r="B9" t="s">
-        <v>461</v>
-      </c>
-      <c r="C9" t="s">
-        <v>460</v>
       </c>
       <c r="D9" t="s">
         <v>15</v>
       </c>
       <c r="E9" t="s">
-        <v>459</v>
-      </c>
-      <c r="H9" t="s">
+        <v>360</v>
+      </c>
+      <c r="I9" s="22">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J9" t="s">
+        <v>432</v>
+      </c>
+      <c r="K9">
+        <v>4.5</v>
+      </c>
+      <c r="L9">
+        <f>A9*K9</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>354</v>
+        <v>456</v>
       </c>
       <c r="C10" t="s">
-        <v>438</v>
+        <v>455</v>
       </c>
       <c r="D10" t="s">
         <v>15</v>
       </c>
       <c r="E10" t="s">
-        <v>363</v>
-      </c>
-      <c r="F10" t="s">
-        <v>355</v>
-      </c>
-      <c r="G10">
-        <v>14</v>
-      </c>
-      <c r="H10">
-        <f>A10*G10</f>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+        <v>463</v>
+      </c>
+      <c r="H10" s="1">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="I10" s="22">
+        <f t="shared" si="0"/>
+        <v>49.800000000000004</v>
+      </c>
+      <c r="L10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>440</v>
+        <v>351</v>
       </c>
       <c r="C11" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="D11" t="s">
         <v>15</v>
       </c>
       <c r="E11" t="s">
-        <v>441</v>
-      </c>
-      <c r="F11" t="s">
-        <v>442</v>
-      </c>
-      <c r="G11">
-        <v>28</v>
-      </c>
-      <c r="H11">
-        <f>A11*G11</f>
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+        <v>360</v>
+      </c>
+      <c r="I11" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J11" t="s">
+        <v>352</v>
+      </c>
+      <c r="K11">
+        <v>14</v>
+      </c>
+      <c r="L11">
+        <f>A11*K11</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>356</v>
+        <v>437</v>
       </c>
       <c r="C12" t="s">
-        <v>367</v>
+        <v>435</v>
       </c>
       <c r="D12" t="s">
         <v>15</v>
       </c>
       <c r="E12" t="s">
-        <v>353</v>
-      </c>
-      <c r="F12" t="s">
-        <v>405</v>
-      </c>
-      <c r="I12">
-        <v>7</v>
-      </c>
-      <c r="J12">
-        <f>A12*I12</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+        <v>464</v>
+      </c>
+      <c r="I12" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J12" t="s">
+        <v>438</v>
+      </c>
+      <c r="K12">
+        <v>28</v>
+      </c>
+      <c r="L12">
+        <f>A12*K12</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>443</v>
+        <v>353</v>
       </c>
       <c r="C13" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="D13" t="s">
         <v>15</v>
       </c>
       <c r="E13" t="s">
-        <v>434</v>
-      </c>
-      <c r="F13" t="s">
-        <v>444</v>
-      </c>
-      <c r="I13">
-        <v>12</v>
-      </c>
-      <c r="J13">
-        <f>A13*I13</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+        <v>464</v>
+      </c>
+      <c r="I13" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J13" t="s">
+        <v>402</v>
+      </c>
+      <c r="M13">
+        <v>7</v>
+      </c>
+      <c r="N13">
+        <f>A13*M13</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>462</v>
+        <v>439</v>
       </c>
       <c r="C14" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D14" t="s">
         <v>15</v>
       </c>
       <c r="E14" t="s">
-        <v>357</v>
-      </c>
-      <c r="H14" t="s">
+        <v>431</v>
+      </c>
+      <c r="I14" s="22">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J14" t="s">
+        <v>440</v>
+      </c>
+      <c r="M14">
+        <v>12</v>
+      </c>
+      <c r="N14">
+        <f>A14*M14</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B15" t="s">
-        <v>358</v>
+        <v>457</v>
       </c>
       <c r="C15" t="s">
-        <v>410</v>
+        <v>362</v>
       </c>
       <c r="D15" t="s">
         <v>15</v>
       </c>
       <c r="E15" t="s">
-        <v>359</v>
-      </c>
-      <c r="F15" t="s">
-        <v>419</v>
-      </c>
-      <c r="H15" t="s">
+        <v>354</v>
+      </c>
+      <c r="H15" s="1">
+        <v>25.34</v>
+      </c>
+      <c r="I15" s="22">
+        <f t="shared" si="0"/>
+        <v>152.04</v>
+      </c>
+      <c r="L15" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="C16" t="s">
-        <v>367</v>
+        <v>407</v>
       </c>
       <c r="D16" t="s">
         <v>15</v>
       </c>
       <c r="E16" t="s">
-        <v>353</v>
-      </c>
-      <c r="F16" t="s">
-        <v>439</v>
-      </c>
-      <c r="I16">
-        <v>2</v>
-      </c>
-      <c r="J16">
-        <f>A16*I16</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+        <v>356</v>
+      </c>
+      <c r="H16" s="1">
+        <v>25</v>
+      </c>
+      <c r="I16" s="22">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="J16" t="s">
+        <v>416</v>
+      </c>
+      <c r="L16" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>456</v>
+        <v>357</v>
       </c>
       <c r="C17" t="s">
-        <v>458</v>
+        <v>364</v>
       </c>
       <c r="D17" t="s">
         <v>15</v>
       </c>
       <c r="E17" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+        <v>350</v>
+      </c>
+      <c r="I17" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J17" t="s">
+        <v>436</v>
+      </c>
+      <c r="M17">
+        <v>2</v>
+      </c>
+      <c r="N17">
+        <f>A17*M17</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>407</v>
+        <v>452</v>
       </c>
       <c r="C18" t="s">
-        <v>406</v>
+        <v>454</v>
       </c>
       <c r="D18" t="s">
         <v>15</v>
       </c>
       <c r="E18" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+        <v>453</v>
+      </c>
+      <c r="H18" s="1">
+        <v>9.7100000000000009</v>
+      </c>
+      <c r="I18" s="22">
+        <f t="shared" si="0"/>
+        <v>19.420000000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B19" t="s">
-        <v>463</v>
+        <v>404</v>
       </c>
       <c r="C19" t="s">
+        <v>403</v>
+      </c>
+      <c r="D19" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" t="s">
+        <v>405</v>
+      </c>
+      <c r="I19" s="22">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E19" t="s">
-        <v>445</v>
-      </c>
-      <c r="F19" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>417</v>
+        <v>465</v>
       </c>
       <c r="C20" t="s">
-        <v>416</v>
-      </c>
-      <c r="F20" t="s">
+        <v>466</v>
+      </c>
+      <c r="E20" t="s">
+        <v>441</v>
+      </c>
+      <c r="I20" s="22">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J20" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>423</v>
+        <v>414</v>
       </c>
       <c r="C21" t="s">
-        <v>422</v>
-      </c>
-      <c r="D21" t="s">
-        <v>421</v>
-      </c>
-      <c r="E21" t="s">
+        <v>413</v>
+      </c>
+      <c r="I21" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J21" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>2</v>
+      </c>
+      <c r="B22" t="s">
         <v>420</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F22" t="s">
-        <v>446</v>
-      </c>
-      <c r="H22">
-        <f>SUM(H2:H21)</f>
+      <c r="C22" t="s">
+        <v>419</v>
+      </c>
+      <c r="D22" t="s">
+        <v>418</v>
+      </c>
+      <c r="E22" t="s">
+        <v>417</v>
+      </c>
+      <c r="H22" s="1">
+        <v>49.41</v>
+      </c>
+      <c r="I22" s="22">
+        <f t="shared" si="0"/>
+        <v>98.82</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I23" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J23" t="s">
+        <v>442</v>
+      </c>
+      <c r="L23">
+        <f>SUM(L2:L22)</f>
         <v>51</v>
       </c>
-      <c r="I22" t="s">
+      <c r="M23" t="s">
         <v>0</v>
       </c>
-      <c r="J22">
-        <f t="shared" ref="J22" si="0">SUM(J2:J21)</f>
+      <c r="N23">
+        <f t="shared" ref="N23" si="1">SUM(N2:N22)</f>
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F23" t="s">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I24" s="22">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H23" t="s">
+      <c r="J24" t="s">
         <v>0</v>
+      </c>
+      <c r="L24" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>1</v>
+      </c>
+      <c r="B25" t="s">
+        <v>461</v>
+      </c>
+      <c r="C25" t="s">
+        <v>435</v>
+      </c>
+      <c r="D25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E25" t="s">
+        <v>360</v>
+      </c>
+      <c r="H25" s="1">
+        <v>96.65</v>
+      </c>
+      <c r="I25" s="22">
+        <f t="shared" si="0"/>
+        <v>96.65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>3</v>
+      </c>
+      <c r="B26" t="s">
+        <v>461</v>
+      </c>
+      <c r="C26" t="s">
+        <v>364</v>
+      </c>
+      <c r="D26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E26" t="s">
+        <v>350</v>
+      </c>
+      <c r="H26" s="1">
+        <v>44.02</v>
+      </c>
+      <c r="I26" s="22">
+        <f t="shared" si="0"/>
+        <v>132.06</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G30" t="s">
+        <v>462</v>
+      </c>
+      <c r="I30" s="1">
+        <f>SUM(I3:I26)</f>
+        <v>1920.6419999999998</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="M1:N1"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3269,7 +3555,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -3277,7 +3563,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>2</v>
@@ -3304,7 +3590,7 @@
         <v>17</v>
       </c>
       <c r="K3" s="10" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -3312,16 +3598,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>271</v>
+      </c>
+      <c r="C4" t="s">
+        <v>273</v>
+      </c>
+      <c r="D4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" t="s">
         <v>274</v>
-      </c>
-      <c r="C4" t="s">
-        <v>276</v>
-      </c>
-      <c r="D4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" t="s">
-        <v>277</v>
       </c>
       <c r="F4" t="s">
         <v>0</v>
@@ -3336,10 +3622,10 @@
         <v>0</v>
       </c>
       <c r="J4" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="K4" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -3347,22 +3633,22 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="C5" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E5" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="J5" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="K5" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -3370,31 +3656,31 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E6" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="F6" t="s">
         <v>15</v>
       </c>
       <c r="G6" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="H6">
         <v>5.61</v>
       </c>
       <c r="J6" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="K6" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -3402,31 +3688,31 @@
         <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C7" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="D7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E7" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="F7" t="s">
         <v>15</v>
       </c>
       <c r="G7" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="H7">
         <v>5.61</v>
       </c>
       <c r="J7" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="K7" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -3434,10 +3720,10 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="C8" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="E8" t="s">
         <v>0</v>
@@ -3446,13 +3732,13 @@
         <v>15</v>
       </c>
       <c r="G8" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="H8">
         <v>20.21</v>
       </c>
       <c r="J8" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
     </row>
   </sheetData>
@@ -3465,8 +3751,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:N25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3488,54 +3774,54 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E3" s="14" t="s">
         <v>3</v>
       </c>
       <c r="F3" s="13" t="s">
+        <v>241</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>242</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="K3" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="L3" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="M3" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="N3" s="10" t="s">
         <v>244</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="H3" s="10" t="s">
-        <v>245</v>
-      </c>
-      <c r="I3" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="J3" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="K3" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="L3" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="M3" s="10" t="s">
-        <v>246</v>
-      </c>
-      <c r="N3" s="10" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -3543,22 +3829,22 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
+        <v>209</v>
+      </c>
+      <c r="D4" t="s">
+        <v>210</v>
+      </c>
+      <c r="E4" t="s">
+        <v>211</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="D4" t="s">
+      <c r="G4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H4" t="s">
         <v>213</v>
-      </c>
-      <c r="E4" t="s">
-        <v>214</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="G4" t="s">
-        <v>44</v>
-      </c>
-      <c r="H4" t="s">
-        <v>216</v>
       </c>
       <c r="I4" s="1">
         <v>2.0499999999999998</v>
@@ -3568,7 +3854,7 @@
         <v>2.0499999999999998</v>
       </c>
       <c r="L4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -3576,22 +3862,22 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D5" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="E5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F5" s="2">
         <v>975</v>
       </c>
       <c r="G5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H5" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="I5" s="1">
         <v>1.1200000000000001</v>
@@ -3601,7 +3887,7 @@
         <v>1.1200000000000001</v>
       </c>
       <c r="L5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -3609,25 +3895,25 @@
         <v>1</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C6" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="D6" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="E6" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="F6" s="2">
         <v>61300411121</v>
       </c>
       <c r="G6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H6" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="I6" s="1">
         <v>0.18</v>
@@ -3637,7 +3923,7 @@
         <v>0.18</v>
       </c>
       <c r="L6" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -3645,22 +3931,22 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D7" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="E7" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="G7" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H7" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="I7" s="1">
         <v>1.44</v>
@@ -3670,7 +3956,7 @@
         <v>1.44</v>
       </c>
       <c r="L7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -3681,22 +3967,22 @@
         <v>0.1</v>
       </c>
       <c r="C8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D8" t="s">
+        <v>302</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F8" t="s">
         <v>84</v>
       </c>
-      <c r="D8" t="s">
-        <v>305</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="F8" t="s">
-        <v>87</v>
-      </c>
       <c r="G8" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H8" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="I8" s="1">
         <v>0.21</v>
@@ -3706,7 +3992,7 @@
         <v>2.1</v>
       </c>
       <c r="L8" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -3714,25 +4000,25 @@
         <v>2</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="C9" t="s">
+        <v>220</v>
+      </c>
+      <c r="D9" t="s">
+        <v>303</v>
+      </c>
+      <c r="E9" t="s">
+        <v>141</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="G9" t="s">
+        <v>41</v>
+      </c>
+      <c r="H9" t="s">
         <v>222</v>
-      </c>
-      <c r="C9" t="s">
-        <v>223</v>
-      </c>
-      <c r="D9" t="s">
-        <v>306</v>
-      </c>
-      <c r="E9" t="s">
-        <v>144</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="G9" t="s">
-        <v>44</v>
-      </c>
-      <c r="H9" t="s">
-        <v>225</v>
       </c>
       <c r="I9" s="1">
         <v>0.72</v>
@@ -3742,7 +4028,7 @@
         <v>1.44</v>
       </c>
       <c r="L9" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -3753,22 +4039,22 @@
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D10" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="E10" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="G10" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H10" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="I10" s="1">
         <v>0.65</v>
@@ -3778,7 +4064,7 @@
         <v>1.3</v>
       </c>
       <c r="L10" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -3789,22 +4075,22 @@
         <v>49.9</v>
       </c>
       <c r="C11" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D11" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="E11" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="G11" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H11" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="I11" s="1">
         <v>0.1</v>
@@ -3814,7 +4100,7 @@
         <v>0.8</v>
       </c>
       <c r="L11" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -3822,25 +4108,25 @@
         <v>3</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="C12" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="D12" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="E12" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="G12" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H12" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="I12" s="1">
         <v>0.36</v>
@@ -3850,7 +4136,7 @@
         <v>1.08</v>
       </c>
       <c r="L12" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -3861,22 +4147,22 @@
         <v>191</v>
       </c>
       <c r="C13" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="D13" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="E13" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="G13" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H13" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="I13" s="1">
         <v>0.1</v>
@@ -3886,7 +4172,7 @@
         <v>0.2</v>
       </c>
       <c r="L13" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -3894,25 +4180,25 @@
         <v>1</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="C14" t="s">
+        <v>316</v>
+      </c>
+      <c r="D14" t="s">
+        <v>307</v>
+      </c>
+      <c r="E14" t="s">
+        <v>181</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="C14" t="s">
-        <v>319</v>
-      </c>
-      <c r="D14" t="s">
-        <v>310</v>
-      </c>
-      <c r="E14" t="s">
-        <v>184</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>321</v>
-      </c>
       <c r="G14" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="I14" s="1">
         <v>0.1</v>
@@ -3922,7 +4208,7 @@
         <v>0.1</v>
       </c>
       <c r="L14" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -3930,25 +4216,25 @@
         <v>1</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C15" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="D15" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="E15" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="G15" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H15" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="I15" s="1">
         <v>0.1</v>
@@ -3958,7 +4244,7 @@
         <v>0.1</v>
       </c>
       <c r="L15" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -3966,25 +4252,25 @@
         <v>4</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="C16" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="D16" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="E16" t="s">
+        <v>426</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="G16" t="s">
+        <v>41</v>
+      </c>
+      <c r="H16" t="s">
         <v>429</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>428</v>
-      </c>
-      <c r="G16" t="s">
-        <v>44</v>
-      </c>
-      <c r="H16" t="s">
-        <v>432</v>
       </c>
       <c r="I16" s="1">
         <v>4.7699999999999996</v>
@@ -3994,7 +4280,7 @@
         <v>19.079999999999998</v>
       </c>
       <c r="L16" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -4002,25 +4288,25 @@
         <v>12</v>
       </c>
       <c r="B17" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="C17" t="s">
+        <v>225</v>
+      </c>
+      <c r="D17" t="s">
+        <v>226</v>
+      </c>
+      <c r="E17" t="s">
         <v>227</v>
       </c>
-      <c r="C17" t="s">
+      <c r="F17" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="D17" t="s">
+      <c r="G17" t="s">
+        <v>41</v>
+      </c>
+      <c r="H17" t="s">
         <v>229</v>
-      </c>
-      <c r="E17" t="s">
-        <v>230</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="G17" t="s">
-        <v>44</v>
-      </c>
-      <c r="H17" t="s">
-        <v>232</v>
       </c>
       <c r="I17" s="1">
         <v>0.91</v>
@@ -4030,7 +4316,7 @@
         <v>10.92</v>
       </c>
       <c r="L17" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -4038,25 +4324,25 @@
         <v>1</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C18" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="D18" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="E18" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="G18" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H18" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="I18" s="1">
         <v>1.28</v>
@@ -4066,7 +4352,7 @@
         <v>1.28</v>
       </c>
       <c r="L18" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -4074,25 +4360,25 @@
         <v>1</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="C19" t="s">
+        <v>234</v>
+      </c>
+      <c r="D19" t="s">
+        <v>235</v>
+      </c>
+      <c r="E19" t="s">
         <v>236</v>
       </c>
-      <c r="C19" t="s">
+      <c r="F19" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="D19" t="s">
+      <c r="G19" t="s">
+        <v>41</v>
+      </c>
+      <c r="H19" t="s">
         <v>238</v>
-      </c>
-      <c r="E19" t="s">
-        <v>239</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="G19" t="s">
-        <v>44</v>
-      </c>
-      <c r="H19" t="s">
-        <v>241</v>
       </c>
       <c r="I19" s="1">
         <v>5.4</v>
@@ -4102,7 +4388,7 @@
         <v>5.4</v>
       </c>
       <c r="L19" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -4110,25 +4396,25 @@
         <v>2</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C20" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="D20" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="E20" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="G20" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H20" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="I20" s="1">
         <v>2.1800000000000002</v>
@@ -4138,7 +4424,7 @@
         <v>4.3600000000000003</v>
       </c>
       <c r="L20" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -4146,25 +4432,25 @@
         <v>2</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C21" t="s">
+        <v>260</v>
+      </c>
+      <c r="D21" t="s">
+        <v>299</v>
+      </c>
+      <c r="E21" t="s">
+        <v>227</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="G21" t="s">
+        <v>41</v>
+      </c>
+      <c r="H21" t="s">
         <v>263</v>
-      </c>
-      <c r="D21" t="s">
-        <v>302</v>
-      </c>
-      <c r="E21" t="s">
-        <v>230</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="G21" t="s">
-        <v>44</v>
-      </c>
-      <c r="H21" t="s">
-        <v>266</v>
       </c>
       <c r="I21" s="1">
         <v>2.64</v>
@@ -4174,7 +4460,7 @@
         <v>5.28</v>
       </c>
       <c r="L21" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -4182,25 +4468,25 @@
         <v>1</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="C22" t="s">
+        <v>264</v>
+      </c>
+      <c r="D22" t="s">
+        <v>299</v>
+      </c>
+      <c r="E22" t="s">
+        <v>227</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="G22" t="s">
+        <v>41</v>
+      </c>
+      <c r="H22" t="s">
         <v>267</v>
-      </c>
-      <c r="D22" t="s">
-        <v>302</v>
-      </c>
-      <c r="E22" t="s">
-        <v>230</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="G22" t="s">
-        <v>44</v>
-      </c>
-      <c r="H22" t="s">
-        <v>270</v>
       </c>
       <c r="I22" s="1">
         <v>1.26</v>
@@ -4210,7 +4496,7 @@
         <v>1.26</v>
       </c>
       <c r="L22" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -4218,22 +4504,22 @@
         <v>1</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="G23" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H23" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="I23" s="1">
         <v>40</v>
@@ -4244,6 +4530,9 @@
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H25" t="s">
+        <v>335</v>
+      </c>
       <c r="J25" s="1">
         <f>SUM(J4:J24)</f>
         <v>99.49</v>
@@ -4259,8 +4548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4EF4737-2343-4468-93BD-3DA932E88D13}">
   <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="J34" sqref="J34"/>
+    <sheetView topLeftCell="B6" workbookViewId="0">
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4280,54 +4569,54 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>3</v>
       </c>
       <c r="F3" t="s">
+        <v>241</v>
+      </c>
+      <c r="G3" t="s">
+        <v>69</v>
+      </c>
+      <c r="H3" t="s">
+        <v>242</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="K3" t="s">
+        <v>72</v>
+      </c>
+      <c r="L3" t="s">
+        <v>73</v>
+      </c>
+      <c r="M3" t="s">
+        <v>243</v>
+      </c>
+      <c r="N3" t="s">
         <v>244</v>
-      </c>
-      <c r="G3" t="s">
-        <v>72</v>
-      </c>
-      <c r="H3" t="s">
-        <v>245</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="K3" t="s">
-        <v>75</v>
-      </c>
-      <c r="L3" t="s">
-        <v>76</v>
-      </c>
-      <c r="M3" t="s">
-        <v>246</v>
-      </c>
-      <c r="N3" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -4338,22 +4627,22 @@
         <v>0</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F4" t="s">
         <v>79</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="G4" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H4" t="s">
         <v>80</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="F4" t="s">
-        <v>82</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H4" t="s">
-        <v>83</v>
       </c>
       <c r="I4" s="1">
         <v>0.16</v>
@@ -4363,7 +4652,7 @@
         <v>1.28</v>
       </c>
       <c r="L4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -4374,22 +4663,22 @@
         <v>0.1</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F5" t="s">
         <v>84</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="G5" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H5" t="s">
         <v>85</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="F5" t="s">
-        <v>87</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H5" t="s">
-        <v>88</v>
       </c>
       <c r="I5" s="1">
         <v>0.21</v>
@@ -4399,7 +4688,7 @@
         <v>2.31</v>
       </c>
       <c r="L5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -4407,25 +4696,25 @@
         <v>9</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F6" t="s">
         <v>89</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="G6" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H6" t="s">
         <v>90</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="F6" t="s">
-        <v>92</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H6" t="s">
-        <v>93</v>
       </c>
       <c r="I6" s="1">
         <v>0.45</v>
@@ -4435,7 +4724,7 @@
         <v>4.05</v>
       </c>
       <c r="L6" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -4443,16 +4732,16 @@
         <v>0</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>0</v>
@@ -4463,7 +4752,7 @@
         <v>0</v>
       </c>
       <c r="K7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="L7" t="s">
         <v>0</v>
@@ -4477,22 +4766,22 @@
         <v>0.22</v>
       </c>
       <c r="C8" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="F8" t="s">
         <v>95</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="G8" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H8" t="s">
         <v>96</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="F8" t="s">
-        <v>98</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H8" t="s">
-        <v>99</v>
       </c>
       <c r="I8" s="1">
         <v>0.78</v>
@@ -4502,7 +4791,7 @@
         <v>6.24</v>
       </c>
       <c r="L8" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="30" x14ac:dyDescent="0.25">
@@ -4513,22 +4802,22 @@
         <v>4.7E-2</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F9" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H9" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I9" s="1">
         <v>0.94</v>
@@ -4538,7 +4827,7 @@
         <v>15.04</v>
       </c>
       <c r="L9" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -4549,22 +4838,22 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="C10" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F10" t="s">
+        <v>102</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H10" t="s">
         <v>103</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>326</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="F10" t="s">
-        <v>105</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H10" t="s">
-        <v>106</v>
       </c>
       <c r="I10" s="1">
         <v>5.44</v>
@@ -4574,7 +4863,7 @@
         <v>43.52</v>
       </c>
       <c r="L10" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -4585,22 +4874,22 @@
         <v>10</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="F11" t="s">
         <v>107</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="G11" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H11" t="s">
         <v>108</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="F11" t="s">
-        <v>110</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H11" t="s">
-        <v>111</v>
       </c>
       <c r="I11" s="1">
         <v>0.54</v>
@@ -4610,7 +4899,7 @@
         <v>2.16</v>
       </c>
       <c r="L11" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -4618,25 +4907,25 @@
         <v>8</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F12" t="s">
+        <v>205</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H12" t="s">
         <v>206</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="F12" t="s">
-        <v>208</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H12" t="s">
-        <v>209</v>
       </c>
       <c r="I12" s="1">
         <v>0.21</v>
@@ -4646,13 +4935,13 @@
         <v>1.68</v>
       </c>
       <c r="L12" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="M12" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="N12" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -4660,25 +4949,25 @@
         <v>8</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="F13" t="s">
         <v>114</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="G13" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H13" t="s">
         <v>115</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="F13" t="s">
-        <v>117</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H13" t="s">
-        <v>118</v>
       </c>
       <c r="I13" s="1">
         <v>0.1</v>
@@ -4688,7 +4977,7 @@
         <v>0.8</v>
       </c>
       <c r="L13" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="45" x14ac:dyDescent="0.25">
@@ -4696,25 +4985,25 @@
         <v>25</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F14" t="s">
         <v>119</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="G14" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H14" t="s">
         <v>120</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="F14" t="s">
-        <v>122</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H14" t="s">
-        <v>123</v>
       </c>
       <c r="I14" s="1">
         <v>0.59</v>
@@ -4724,7 +5013,7 @@
         <v>14.75</v>
       </c>
       <c r="L14" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -4732,25 +5021,25 @@
         <v>8</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F15" t="s">
         <v>124</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="G15" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H15" t="s">
         <v>125</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="F15" t="s">
-        <v>127</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H15" t="s">
-        <v>128</v>
       </c>
       <c r="I15" s="1">
         <v>0.59</v>
@@ -4760,7 +5049,7 @@
         <v>4.72</v>
       </c>
       <c r="L15" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="30" x14ac:dyDescent="0.25">
@@ -4768,25 +5057,25 @@
         <v>16</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="F16" t="s">
         <v>130</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="G16" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H16" t="s">
         <v>131</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="F16" t="s">
-        <v>133</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H16" t="s">
-        <v>134</v>
       </c>
       <c r="I16" s="1">
         <v>0.68</v>
@@ -4796,7 +5085,7 @@
         <v>10.88</v>
       </c>
       <c r="L16" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -4804,25 +5093,25 @@
         <v>1</v>
       </c>
       <c r="B17" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="F17" t="s">
         <v>136</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="G17" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H17" t="s">
         <v>137</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="F17" t="s">
-        <v>139</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H17" t="s">
-        <v>140</v>
       </c>
       <c r="I17" s="1">
         <v>2.0699999999999998</v>
@@ -4840,25 +5129,25 @@
         <v>1</v>
       </c>
       <c r="B18" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="E18" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="F18" t="s">
         <v>142</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="G18" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H18" t="s">
         <v>143</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="F18" t="s">
-        <v>145</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H18" t="s">
-        <v>146</v>
       </c>
       <c r="I18" s="1">
         <v>0.66</v>
@@ -4876,25 +5165,25 @@
         <v>1</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="E19" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="F19" t="s">
         <v>148</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="G19" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H19" t="s">
         <v>149</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="F19" t="s">
-        <v>151</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H19" t="s">
-        <v>152</v>
       </c>
       <c r="I19" s="1">
         <v>18.47</v>
@@ -4912,25 +5201,25 @@
         <v>8</v>
       </c>
       <c r="B20" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="E20" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="F20" t="s">
         <v>154</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="G20" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H20" t="s">
         <v>155</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="F20" t="s">
-        <v>157</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H20" t="s">
-        <v>158</v>
       </c>
       <c r="I20" s="1">
         <v>2.29</v>
@@ -4948,25 +5237,25 @@
         <v>8</v>
       </c>
       <c r="B21" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="F21" t="s">
         <v>165</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="G21" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H21" t="s">
         <v>166</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="F21" t="s">
-        <v>168</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H21" t="s">
-        <v>169</v>
       </c>
       <c r="I21" s="1">
         <v>2.73</v>
@@ -4984,25 +5273,25 @@
         <v>8</v>
       </c>
       <c r="B22" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="E22" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="F22" t="s">
         <v>171</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="G22" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H22" t="s">
         <v>172</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="F22" t="s">
-        <v>174</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H22" t="s">
-        <v>175</v>
       </c>
       <c r="I22" s="1">
         <v>0.18</v>
@@ -5012,7 +5301,7 @@
         <v>1.44</v>
       </c>
       <c r="L22" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
@@ -5020,25 +5309,25 @@
         <v>9</v>
       </c>
       <c r="B23" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="E23" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="F23" t="s">
         <v>177</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="G23" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H23" t="s">
         <v>178</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="F23" t="s">
-        <v>180</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H23" t="s">
-        <v>181</v>
       </c>
       <c r="I23" s="1">
         <v>0.81</v>
@@ -5048,7 +5337,7 @@
         <v>7.2900000000000009</v>
       </c>
       <c r="L23" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
@@ -5059,22 +5348,22 @@
         <v>499</v>
       </c>
       <c r="C24" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="F24" t="s">
         <v>182</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="G24" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H24" t="s">
         <v>183</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="F24" t="s">
-        <v>185</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H24" t="s">
-        <v>186</v>
       </c>
       <c r="I24" s="1">
         <v>0.1</v>
@@ -5084,7 +5373,7 @@
         <v>0.8</v>
       </c>
       <c r="L24" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
@@ -5095,22 +5384,22 @@
         <v>10</v>
       </c>
       <c r="C25" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="F25" t="s">
+        <v>186</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H25" t="s">
         <v>187</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="F25" t="s">
-        <v>189</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H25" t="s">
-        <v>190</v>
       </c>
       <c r="I25" s="1">
         <v>0.1</v>
@@ -5120,7 +5409,7 @@
         <v>0.1</v>
       </c>
       <c r="L25" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
@@ -5128,26 +5417,29 @@
         <v>1</v>
       </c>
       <c r="C26" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F26" t="s">
+        <v>368</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="H26" s="18" t="s">
+        <v>369</v>
+      </c>
+      <c r="I26" s="1">
+        <v>15</v>
+      </c>
+      <c r="J26" s="1">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="M26" t="s">
         <v>192</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F26" t="s">
-        <v>371</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="H26" s="18" t="s">
-        <v>372</v>
-      </c>
-      <c r="J26" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M26" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
@@ -5155,22 +5447,22 @@
         <v>8</v>
       </c>
       <c r="C27" t="s">
+        <v>421</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>422</v>
+      </c>
+      <c r="F27" t="s">
+        <v>423</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H27" t="s">
         <v>424</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>332</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>425</v>
-      </c>
-      <c r="F27" t="s">
-        <v>426</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H27" t="s">
-        <v>427</v>
       </c>
       <c r="I27" s="1">
         <v>0.1</v>
@@ -5185,25 +5477,25 @@
         <v>8</v>
       </c>
       <c r="B29" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="E29" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="F29" t="s">
         <v>160</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="G29" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H29" t="s">
         <v>161</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="F29" t="s">
-        <v>163</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H29" t="s">
-        <v>164</v>
       </c>
       <c r="I29" s="1">
         <v>2.2400000000000002</v>
@@ -5219,7 +5511,7 @@
         <v>0</v>
       </c>
       <c r="M29" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
@@ -5233,7 +5525,7 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="3"/>
@@ -5243,7 +5535,7 @@
       <c r="I31" s="1"/>
       <c r="J31" s="1">
         <f>SUM(J4:J30)</f>
-        <v>197.14</v>
+        <v>212.14</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -5251,30 +5543,30 @@
         <v>0</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F32" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="M32" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="33" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C33" s="3" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F33" t="s">
+        <v>195</v>
+      </c>
+      <c r="M33" t="s">
         <v>198</v>
-      </c>
-      <c r="M33" t="s">
-        <v>201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update print files and BOM
Change diffuser to 1/8" not 1/16"
</commit_message>
<xml_diff>
--- a/96ChannelRecordingRig.xlsx
+++ b/96ChannelRecordingRig.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sawtelles\Documents\GitHub\FlySong\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D315ECBE-0D4A-4043-95E0-3C292D755ABD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06317C91-FF8F-4048-8E97-5918A3125E1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="18240" windowHeight="28320" xr2:uid="{0B008E79-2D1D-4383-A393-19DDE4F60BB8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" firstSheet="1" activeTab="2" xr2:uid="{0B008E79-2D1D-4383-A393-19DDE4F60BB8}"/>
   </bookViews>
   <sheets>
     <sheet name="Top Level" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="470">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -1288,9 +1288,6 @@
     <t>Serial cable assembly</t>
   </si>
   <si>
-    <t xml:space="preserve"> 2447 White 1/16" thick</t>
-  </si>
-  <si>
     <t>Laser Cut using FlySongRGBMirror.dxf</t>
   </si>
   <si>
@@ -1442,6 +1439,18 @@
   </si>
   <si>
     <t>3-D printed</t>
+  </si>
+  <si>
+    <t>AE4E25E</t>
+  </si>
+  <si>
+    <t>Adapter with Internal 4-40 Threads and External 1/4"-20 Thread</t>
+  </si>
+  <si>
+    <t>Thread adapter</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2447 White 1/18" thick</t>
   </si>
 </sst>
 </file>
@@ -1559,9 +1568,6 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1570,6 +1576,9 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1889,8 +1898,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E3" workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="42.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2009,25 +2018,25 @@
         <v>108.16</v>
       </c>
       <c r="J5" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D6" t="s">
         <v>412</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="I6" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J6" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -2359,7 +2368,7 @@
         <v>56</v>
       </c>
       <c r="F18" t="s">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="G18" s="9" t="s">
         <v>10</v>
@@ -2419,7 +2428,7 @@
         <v>410</v>
       </c>
       <c r="F20" t="s">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="G20" s="9" t="s">
         <v>10</v>
@@ -2563,12 +2572,12 @@
         <v>339</v>
       </c>
       <c r="H27" s="1">
-        <f>'RGB-IR Lighting'!$I$30</f>
-        <v>1920.6419999999998</v>
+        <f>'RGB-IR Lighting'!$I$31</f>
+        <v>2189.0219999999995</v>
       </c>
       <c r="I27" s="1">
         <f t="shared" si="0"/>
-        <v>1920.6419999999998</v>
+        <v>2189.0219999999995</v>
       </c>
       <c r="J27" t="s">
         <v>340</v>
@@ -2580,7 +2589,7 @@
       </c>
       <c r="I29" s="1">
         <f>SUM(I4:I27)</f>
-        <v>11612.082</v>
+        <v>11880.462</v>
       </c>
     </row>
   </sheetData>
@@ -2594,7 +2603,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2810,10 +2819,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE26C6C8-A75F-4B07-BB7A-B53D3B568C33}">
-  <dimension ref="A1:T30"/>
+  <dimension ref="A1:T31"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2838,14 +2847,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="K1" s="19" t="s">
+      <c r="K1" s="22" t="s">
+        <v>446</v>
+      </c>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22" t="s">
         <v>447</v>
       </c>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19" t="s">
-        <v>448</v>
-      </c>
-      <c r="N1" s="19"/>
+      <c r="N1" s="22"/>
     </row>
     <row r="2" spans="1:20" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
@@ -2869,26 +2878,26 @@
       <c r="G2" s="13" t="s">
         <v>378</v>
       </c>
-      <c r="H2" s="21" t="s">
+      <c r="H2" s="20" t="s">
+        <v>457</v>
+      </c>
+      <c r="I2" s="13" t="s">
         <v>458</v>
-      </c>
-      <c r="I2" s="13" t="s">
-        <v>459</v>
       </c>
       <c r="J2" s="10" t="s">
         <v>17</v>
       </c>
       <c r="K2" s="10" t="s">
+        <v>448</v>
+      </c>
+      <c r="L2" s="10" t="s">
         <v>449</v>
       </c>
-      <c r="L2" s="10" t="s">
-        <v>450</v>
-      </c>
       <c r="M2" s="10" t="s">
+        <v>448</v>
+      </c>
+      <c r="N2" s="10" t="s">
         <v>449</v>
-      </c>
-      <c r="N2" s="10" t="s">
-        <v>450</v>
       </c>
       <c r="O2" s="12" t="s">
         <v>70</v>
@@ -2922,10 +2931,10 @@
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
-      <c r="H3" s="20">
+      <c r="H3" s="19">
         <v>298.75599999999997</v>
       </c>
-      <c r="I3" s="22">
+      <c r="I3" s="21">
         <f>H3*A3</f>
         <v>597.51199999999994</v>
       </c>
@@ -2937,16 +2946,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
-      <c r="H4" s="20">
+      <c r="H4" s="19">
         <v>90.11</v>
       </c>
-      <c r="I4" s="22">
-        <f t="shared" ref="I4:I26" si="0">H4*A4</f>
+      <c r="I4" s="21">
+        <f t="shared" ref="I4:I27" si="0">H4*A4</f>
         <v>180.22</v>
       </c>
       <c r="O4" s="1"/>
@@ -2971,7 +2980,7 @@
       <c r="H5" s="1">
         <v>172.4</v>
       </c>
-      <c r="I5" s="22">
+      <c r="I5" s="21">
         <f t="shared" si="0"/>
         <v>344.8</v>
       </c>
@@ -2981,78 +2990,71 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2</v>
+        <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>344</v>
+        <v>468</v>
+      </c>
+      <c r="C6" t="s">
+        <v>467</v>
       </c>
       <c r="D6" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="E6" t="s">
-        <v>415</v>
-      </c>
-      <c r="I6" s="22">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J6" t="s">
-        <v>451</v>
+        <v>466</v>
+      </c>
+      <c r="H6">
+        <v>4.97</v>
+      </c>
+      <c r="I6" s="21">
+        <f t="shared" si="0"/>
+        <v>268.38</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>349</v>
-      </c>
-      <c r="C7" t="s">
-        <v>406</v>
+        <v>344</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>345</v>
       </c>
       <c r="E7" t="s">
-        <v>348</v>
-      </c>
-      <c r="H7" s="1">
-        <v>49.83</v>
-      </c>
-      <c r="I7" s="22">
-        <f t="shared" si="0"/>
-        <v>199.32</v>
+        <v>469</v>
+      </c>
+      <c r="I7" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J7" t="s">
+        <v>450</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>433</v>
+        <v>349</v>
       </c>
       <c r="C8" t="s">
-        <v>364</v>
+        <v>406</v>
       </c>
       <c r="D8" t="s">
         <v>15</v>
       </c>
       <c r="E8" t="s">
-        <v>350</v>
-      </c>
-      <c r="I8" s="22">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J8" t="s">
-        <v>432</v>
-      </c>
-      <c r="M8">
-        <v>4.5</v>
-      </c>
-      <c r="N8">
-        <f>A8*M8</f>
-        <v>9</v>
+        <v>348</v>
+      </c>
+      <c r="H8" s="1">
+        <v>49.83</v>
+      </c>
+      <c r="I8" s="21">
+        <f t="shared" si="0"/>
+        <v>199.32</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
@@ -3060,88 +3062,88 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C9" t="s">
-        <v>435</v>
+        <v>364</v>
       </c>
       <c r="D9" t="s">
         <v>15</v>
       </c>
       <c r="E9" t="s">
-        <v>360</v>
-      </c>
-      <c r="I9" s="22">
+        <v>350</v>
+      </c>
+      <c r="I9" s="21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J9" t="s">
-        <v>432</v>
-      </c>
-      <c r="K9">
+        <v>431</v>
+      </c>
+      <c r="M9">
         <v>4.5</v>
       </c>
-      <c r="L9">
-        <f>A9*K9</f>
+      <c r="N9">
+        <f>A9*M9</f>
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>456</v>
+        <v>433</v>
       </c>
       <c r="C10" t="s">
-        <v>455</v>
+        <v>434</v>
       </c>
       <c r="D10" t="s">
         <v>15</v>
       </c>
       <c r="E10" t="s">
-        <v>463</v>
-      </c>
-      <c r="H10" s="1">
-        <v>16.600000000000001</v>
-      </c>
-      <c r="I10" s="22">
-        <f t="shared" si="0"/>
-        <v>49.800000000000004</v>
-      </c>
-      <c r="L10" t="s">
+        <v>360</v>
+      </c>
+      <c r="I10" s="21">
+        <f t="shared" si="0"/>
         <v>0</v>
+      </c>
+      <c r="J10" t="s">
+        <v>431</v>
+      </c>
+      <c r="K10">
+        <v>4.5</v>
+      </c>
+      <c r="L10">
+        <f>A10*K10</f>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>351</v>
+        <v>455</v>
       </c>
       <c r="C11" t="s">
-        <v>435</v>
+        <v>454</v>
       </c>
       <c r="D11" t="s">
         <v>15</v>
       </c>
       <c r="E11" t="s">
-        <v>360</v>
-      </c>
-      <c r="I11" s="22">
-        <f t="shared" si="0"/>
+        <v>462</v>
+      </c>
+      <c r="H11" s="1">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="I11" s="21">
+        <f t="shared" si="0"/>
+        <v>49.800000000000004</v>
+      </c>
+      <c r="L11" t="s">
         <v>0</v>
-      </c>
-      <c r="J11" t="s">
-        <v>352</v>
-      </c>
-      <c r="K11">
-        <v>14</v>
-      </c>
-      <c r="L11">
-        <f>A11*K11</f>
-        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
@@ -3149,30 +3151,30 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>437</v>
+        <v>351</v>
       </c>
       <c r="C12" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D12" t="s">
         <v>15</v>
       </c>
       <c r="E12" t="s">
-        <v>464</v>
-      </c>
-      <c r="I12" s="22">
+        <v>360</v>
+      </c>
+      <c r="I12" s="21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J12" t="s">
-        <v>438</v>
+        <v>352</v>
       </c>
       <c r="K12">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="L12">
         <f>A12*K12</f>
-        <v>28</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
@@ -3180,30 +3182,30 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>353</v>
+        <v>436</v>
       </c>
       <c r="C13" t="s">
-        <v>364</v>
+        <v>434</v>
       </c>
       <c r="D13" t="s">
         <v>15</v>
       </c>
       <c r="E13" t="s">
-        <v>464</v>
-      </c>
-      <c r="I13" s="22">
+        <v>463</v>
+      </c>
+      <c r="I13" s="21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J13" t="s">
-        <v>402</v>
-      </c>
-      <c r="M13">
-        <v>7</v>
-      </c>
-      <c r="N13">
-        <f>A13*M13</f>
-        <v>7</v>
+        <v>437</v>
+      </c>
+      <c r="K13">
+        <v>28</v>
+      </c>
+      <c r="L13">
+        <f>A13*K13</f>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
@@ -3211,7 +3213,7 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>439</v>
+        <v>353</v>
       </c>
       <c r="C14" t="s">
         <v>364</v>
@@ -3220,75 +3222,76 @@
         <v>15</v>
       </c>
       <c r="E14" t="s">
-        <v>431</v>
-      </c>
-      <c r="I14" s="22">
+        <v>463</v>
+      </c>
+      <c r="I14" s="21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J14" t="s">
-        <v>440</v>
+        <v>402</v>
       </c>
       <c r="M14">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="N14">
         <f>A14*M14</f>
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>457</v>
+        <v>438</v>
       </c>
       <c r="C15" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="D15" t="s">
         <v>15</v>
       </c>
       <c r="E15" t="s">
-        <v>354</v>
-      </c>
-      <c r="H15" s="1">
-        <v>25.34</v>
-      </c>
-      <c r="I15" s="22">
-        <f t="shared" si="0"/>
-        <v>152.04</v>
-      </c>
-      <c r="L15" t="s">
+        <v>430</v>
+      </c>
+      <c r="I15" s="21">
+        <f t="shared" si="0"/>
         <v>0</v>
+      </c>
+      <c r="J15" t="s">
+        <v>439</v>
+      </c>
+      <c r="M15">
+        <v>12</v>
+      </c>
+      <c r="N15">
+        <f>A15*M15</f>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B16" t="s">
-        <v>355</v>
+        <v>456</v>
       </c>
       <c r="C16" t="s">
-        <v>407</v>
+        <v>362</v>
       </c>
       <c r="D16" t="s">
         <v>15</v>
       </c>
       <c r="E16" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="H16" s="1">
-        <v>25</v>
-      </c>
-      <c r="I16" s="22">
-        <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-      <c r="J16" t="s">
-        <v>416</v>
+        <v>25.34</v>
+      </c>
+      <c r="I16" s="21">
+        <f t="shared" si="0"/>
+        <v>152.04</v>
       </c>
       <c r="L16" t="s">
         <v>0</v>
@@ -3299,30 +3302,29 @@
         <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C17" t="s">
-        <v>364</v>
+        <v>407</v>
       </c>
       <c r="D17" t="s">
         <v>15</v>
       </c>
       <c r="E17" t="s">
-        <v>350</v>
-      </c>
-      <c r="I17" s="22">
-        <f t="shared" si="0"/>
+        <v>356</v>
+      </c>
+      <c r="H17" s="1">
+        <v>25</v>
+      </c>
+      <c r="I17" s="21">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="J17" t="s">
+        <v>415</v>
+      </c>
+      <c r="L17" t="s">
         <v>0</v>
-      </c>
-      <c r="J17" t="s">
-        <v>436</v>
-      </c>
-      <c r="M17">
-        <v>2</v>
-      </c>
-      <c r="N17">
-        <f>A17*M17</f>
-        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
@@ -3330,65 +3332,75 @@
         <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>452</v>
+        <v>357</v>
       </c>
       <c r="C18" t="s">
-        <v>454</v>
+        <v>364</v>
       </c>
       <c r="D18" t="s">
         <v>15</v>
       </c>
       <c r="E18" t="s">
-        <v>453</v>
-      </c>
-      <c r="H18" s="1">
-        <v>9.7100000000000009</v>
-      </c>
-      <c r="I18" s="22">
-        <f t="shared" si="0"/>
-        <v>19.420000000000002</v>
+        <v>350</v>
+      </c>
+      <c r="I18" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J18" t="s">
+        <v>435</v>
+      </c>
+      <c r="M18">
+        <v>2</v>
+      </c>
+      <c r="N18">
+        <f>A18*M18</f>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>404</v>
+        <v>451</v>
       </c>
       <c r="C19" t="s">
-        <v>403</v>
+        <v>453</v>
       </c>
       <c r="D19" t="s">
         <v>15</v>
       </c>
       <c r="E19" t="s">
-        <v>405</v>
-      </c>
-      <c r="I19" s="22">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>452</v>
+      </c>
+      <c r="H19" s="1">
+        <v>9.7100000000000009</v>
+      </c>
+      <c r="I19" s="21">
+        <f t="shared" si="0"/>
+        <v>19.420000000000002</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B20" t="s">
-        <v>465</v>
+        <v>404</v>
       </c>
       <c r="C20" t="s">
-        <v>466</v>
+        <v>403</v>
+      </c>
+      <c r="D20" t="s">
+        <v>15</v>
       </c>
       <c r="E20" t="s">
-        <v>441</v>
-      </c>
-      <c r="I20" s="22">
+        <v>405</v>
+      </c>
+      <c r="I20" s="21">
         <f t="shared" si="0"/>
         <v>0</v>
-      </c>
-      <c r="J20" t="s">
-        <v>412</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
@@ -3396,17 +3408,20 @@
         <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>414</v>
+        <v>464</v>
       </c>
       <c r="C21" t="s">
-        <v>413</v>
-      </c>
-      <c r="I21" s="22">
+        <v>465</v>
+      </c>
+      <c r="E21" t="s">
+        <v>440</v>
+      </c>
+      <c r="I21" s="21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J21" t="s">
-        <v>0</v>
+        <v>412</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
@@ -3414,112 +3429,136 @@
         <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>420</v>
+        <v>414</v>
       </c>
       <c r="C22" t="s">
+        <v>413</v>
+      </c>
+      <c r="I22" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J22" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>2</v>
+      </c>
+      <c r="B23" t="s">
         <v>419</v>
       </c>
-      <c r="D22" t="s">
+      <c r="C23" t="s">
         <v>418</v>
       </c>
-      <c r="E22" t="s">
+      <c r="D23" t="s">
         <v>417</v>
       </c>
-      <c r="H22" s="1">
+      <c r="E23" t="s">
+        <v>416</v>
+      </c>
+      <c r="H23" s="1">
         <v>49.41</v>
       </c>
-      <c r="I22" s="22">
+      <c r="I23" s="21">
         <f t="shared" si="0"/>
         <v>98.82</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="I23" s="22">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I24" s="21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J23" t="s">
-        <v>442</v>
-      </c>
-      <c r="L23">
-        <f>SUM(L2:L22)</f>
+      <c r="J24" t="s">
+        <v>441</v>
+      </c>
+      <c r="L24">
+        <f>SUM(L2:L23)</f>
         <v>51</v>
       </c>
-      <c r="M23" t="s">
+      <c r="M24" t="s">
         <v>0</v>
       </c>
-      <c r="N23">
-        <f t="shared" ref="N23" si="1">SUM(N2:N22)</f>
+      <c r="N24">
+        <f t="shared" ref="N24" si="1">SUM(N2:N23)</f>
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="I24" s="22">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I25" s="21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J24" t="s">
+      <c r="J25" t="s">
         <v>0</v>
       </c>
-      <c r="L24" t="s">
+      <c r="L25" t="s">
         <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>1</v>
-      </c>
-      <c r="B25" t="s">
-        <v>461</v>
-      </c>
-      <c r="C25" t="s">
-        <v>435</v>
-      </c>
-      <c r="D25" t="s">
-        <v>15</v>
-      </c>
-      <c r="E25" t="s">
-        <v>360</v>
-      </c>
-      <c r="H25" s="1">
-        <v>96.65</v>
-      </c>
-      <c r="I25" s="22">
-        <f t="shared" si="0"/>
-        <v>96.65</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C26" t="s">
-        <v>364</v>
+        <v>434</v>
       </c>
       <c r="D26" t="s">
         <v>15</v>
       </c>
       <c r="E26" t="s">
+        <v>360</v>
+      </c>
+      <c r="H26" s="1">
+        <v>96.65</v>
+      </c>
+      <c r="I26" s="21">
+        <f t="shared" si="0"/>
+        <v>96.65</v>
+      </c>
+      <c r="L26">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>3</v>
+      </c>
+      <c r="B27" t="s">
+        <v>460</v>
+      </c>
+      <c r="C27" t="s">
+        <v>364</v>
+      </c>
+      <c r="D27" t="s">
+        <v>15</v>
+      </c>
+      <c r="E27" t="s">
         <v>350</v>
       </c>
-      <c r="H26" s="1">
+      <c r="H27" s="1">
         <v>44.02</v>
       </c>
-      <c r="I26" s="22">
+      <c r="I27" s="21">
         <f t="shared" si="0"/>
         <v>132.06</v>
       </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G30" t="s">
-        <v>462</v>
-      </c>
-      <c r="I30" s="1">
-        <f>SUM(I3:I26)</f>
-        <v>1920.6419999999998</v>
+      <c r="N27">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G31" t="s">
+        <v>461</v>
+      </c>
+      <c r="I31" s="1">
+        <f>SUM(I3:I27)</f>
+        <v>2189.0219999999995</v>
       </c>
     </row>
   </sheetData>
@@ -3538,7 +3577,7 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3751,8 +3790,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:N25"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView topLeftCell="B13" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3877,7 +3916,7 @@
         <v>41</v>
       </c>
       <c r="H5" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="I5" s="1">
         <v>1.1200000000000001</v>
@@ -4252,25 +4291,25 @@
         <v>4</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C16" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D16" t="s">
         <v>311</v>
       </c>
       <c r="E16" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="G16" t="s">
         <v>41</v>
       </c>
       <c r="H16" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="I16" s="1">
         <v>4.7699999999999996</v>
@@ -4548,7 +4587,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4EF4737-2343-4468-93BD-3DA932E88D13}">
   <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView topLeftCell="B6" workbookViewId="0">
+    <sheetView topLeftCell="B16" workbookViewId="0">
       <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
@@ -5447,22 +5486,22 @@
         <v>8</v>
       </c>
       <c r="C27" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>329</v>
       </c>
       <c r="E27" s="3" t="s">
+        <v>421</v>
+      </c>
+      <c r="F27" t="s">
         <v>422</v>
-      </c>
-      <c r="F27" t="s">
-        <v>423</v>
       </c>
       <c r="G27" s="3" t="s">
         <v>74</v>
       </c>
       <c r="H27" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="I27" s="1">
         <v>0.1</v>

</xml_diff>